<commit_message>
Update Excel a Texto
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" state="visible" r:id="rId2"/>
@@ -96,14 +96,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,6 +127,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -196,7 +199,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -205,11 +208,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -303,42 +314,42 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,29 +395,29 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="AMJ1" s="0"/>
@@ -418,10 +429,10 @@
       <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="2" t="n">
         <v>34073329</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <v>1160444719</v>
       </c>
     </row>
@@ -432,17 +443,17 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2" t="n">
         <v>3245678</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="2" t="n">
         <v>1157572274</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -457,30 +468,30 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.79"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="AMJ1" s="0"/>
@@ -496,7 +507,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -512,29 +523,29 @@
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="14.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
       <c r="AMJ1" s="0"/>
@@ -546,14 +557,14 @@
       <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="2" t="n">
         <v>543416869777</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -568,30 +579,30 @@
   </sheetPr>
   <dimension ref="A1:AMJ2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.79"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="3"/>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -608,7 +619,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
Se Actualiza el Archivo Cuenta
Se Eliminia Marco Tech de Tech.
Se Elimina cuenta duplicada en Sales.
Se Agrega Cuenta en Marketing.
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20115" windowHeight="7770" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20115" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>Descripción</t>
   </si>
@@ -109,10 +109,10 @@
     <t>(*)N.º Línea</t>
   </si>
   <si>
-    <t>Marcos Tech</t>
-  </si>
-  <si>
-    <t>ContactNew TestP</t>
+    <t>Cuenta sin Servicio</t>
+  </si>
+  <si>
+    <t>aaaaCuenta Activa S/Serv</t>
   </si>
 </sst>
 </file>
@@ -194,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,6 +212,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,11 +493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C995" sqref="C995"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -574,6 +575,14 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -586,10 +595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -676,20 +685,6 @@
         <v>19</v>
       </c>
       <c r="D4" s="7"/>
-    </row>
-    <row r="5" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="7">
-        <v>3245678</v>
-      </c>
-      <c r="D5" s="7">
-        <v>1157572274</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
@@ -776,10 +771,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -840,17 +835,6 @@
         <v>543416869777</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3">
-        <v>22112211</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -865,7 +849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sales 2 newacc Sales
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\telecom2\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20115" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20112" windowHeight="7776" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Descripción</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>aaaaCuenta Activa S/Serv</t>
+  </si>
+  <si>
+    <t>aaaaRaul Care</t>
+  </si>
+  <si>
+    <t>Cuenta con gestiones</t>
   </si>
 </sst>
 </file>
@@ -495,21 +501,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +551,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -555,7 +561,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -565,7 +571,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -575,7 +581,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -595,22 +601,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -646,7 +652,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -660,7 +666,7 @@
         <v>1160444719</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -674,7 +680,7 @@
         <v>1157572274</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
@@ -685,6 +691,14 @@
         <v>19</v>
       </c>
       <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
@@ -704,16 +718,16 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +763,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -777,17 +791,17 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,7 +837,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -853,16 +867,16 @@
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,7 +910,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
camios en sales + add cliente blacklist en cuentas
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\telecom2\TelecomProyectoFAN\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20115" windowHeight="7770"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -19,11 +14,12 @@
     <sheet name="SCP" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:I4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Descripción</t>
   </si>
@@ -113,13 +109,19 @@
   </si>
   <si>
     <t>aaaaCuenta Activa S/Serv</t>
+  </si>
+  <si>
+    <t>Blacklist</t>
+  </si>
+  <si>
+    <t>Prueba Fraude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -137,6 +139,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -194,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,6 +220,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -595,10 +603,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -686,9 +694,20 @@
       </c>
       <c r="D4" s="7"/>
     </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>22355504</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>

</xml_diff>

<commit_message>
nominaciones y sales 2
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -3,8 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14208" windowHeight="1620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -14,12 +19,11 @@
     <sheet name="SCP" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Descripción</t>
   </si>
@@ -115,6 +119,12 @@
   </si>
   <si>
     <t>Prueba Fraude</t>
+  </si>
+  <si>
+    <t>Cliente Wholesale</t>
+  </si>
+  <si>
+    <t>Cuenta Bolsa</t>
   </si>
 </sst>
 </file>
@@ -508,16 +518,16 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +563,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -563,7 +573,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -573,7 +583,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -583,7 +593,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -603,22 +613,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,7 +664,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -668,7 +678,7 @@
         <v>1160444719</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -682,7 +692,7 @@
         <v>1157572274</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
@@ -694,7 +704,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -703,6 +713,17 @@
       </c>
       <c r="C5">
         <v>22355504</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>10000018</v>
       </c>
     </row>
   </sheetData>
@@ -723,16 +744,16 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -768,7 +789,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -796,17 +817,17 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,7 +863,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -872,16 +893,16 @@
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,7 +936,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Revert "configuracion para alta de lineas masivas"
This reverts commit 3a2c6a8be93d8c51bbae3d30a368c0b91393efe9.
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florangel\git\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14208" windowHeight="1620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,13 @@
     <sheet name="Customer" sheetId="3" r:id="rId3"/>
     <sheet name="Tech" sheetId="4" r:id="rId4"/>
     <sheet name="SCP" sheetId="5" r:id="rId5"/>
-    <sheet name="AltaMasiva" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Descripción</t>
   </si>
@@ -126,106 +125,13 @@
   </si>
   <si>
     <t>Cuenta Bolsa</t>
-  </si>
-  <si>
-    <t>Alta de Linea</t>
-  </si>
-  <si>
-    <t>Plan</t>
-  </si>
-  <si>
-    <t>IVA</t>
-  </si>
-  <si>
-    <t>Provincia</t>
-  </si>
-  <si>
-    <t>Plan con Tarjeta Repro </t>
-  </si>
-  <si>
-    <t>IVA Consumidor Final</t>
-  </si>
-  <si>
-    <t>Buenos Aires</t>
-  </si>
-  <si>
-    <t>Plan Prepago Nacional</t>
-  </si>
-  <si>
-    <t>CABA</t>
-  </si>
-  <si>
-    <t>Chaco</t>
-  </si>
-  <si>
-    <t>Chubut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Córdoba </t>
-  </si>
-  <si>
-    <t>Corrientes</t>
-  </si>
-  <si>
-    <t>Entre Ríos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formosa </t>
-  </si>
-  <si>
-    <t>Jujuy</t>
-  </si>
-  <si>
-    <t>La Rioja</t>
-  </si>
-  <si>
-    <t>Mendoza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Misiones </t>
-  </si>
-  <si>
-    <t>Neuquén</t>
-  </si>
-  <si>
-    <t>Rio Negro</t>
-  </si>
-  <si>
-    <t>Salta</t>
-  </si>
-  <si>
-    <t>San Juan</t>
-  </si>
-  <si>
-    <t>Santa Cruz</t>
-  </si>
-  <si>
-    <t>Santa Fe</t>
-  </si>
-  <si>
-    <t>Sgo. Del Estero</t>
-  </si>
-  <si>
-    <t>Tierra del Fuego</t>
-  </si>
-  <si>
-    <t>Tucumán</t>
-  </si>
-  <si>
-    <t>Catamarca</t>
-  </si>
-  <si>
-    <t>La Pampa</t>
-  </si>
-  <si>
-    <t>San Luis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -249,13 +155,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,20 +169,8 @@
         <bgColor rgb="FFF3715A"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD99594"/>
-        <bgColor rgb="FFD99594"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB8CCE4"/>
-        <bgColor rgb="FFB8CCE4"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -318,27 +207,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -358,12 +231,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -648,16 +518,16 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +563,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -703,7 +573,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -713,7 +583,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -723,7 +593,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -745,20 +615,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -794,7 +664,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -808,7 +678,7 @@
         <v>1160444719</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -822,7 +692,7 @@
         <v>1157572274</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
@@ -834,7 +704,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -845,7 +715,7 @@
         <v>22355504</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -874,16 +744,16 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -919,7 +789,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -947,17 +817,17 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -993,7 +863,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1023,16 +893,16 @@
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1066,7 +936,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1085,407 +955,4 @@
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W26"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-    </row>
-    <row r="2" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>34</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
configuracion para alta de lineas masivas
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florangel\git\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14208" windowHeight="1620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Customer" sheetId="3" r:id="rId3"/>
     <sheet name="Tech" sheetId="4" r:id="rId4"/>
     <sheet name="SCP" sheetId="5" r:id="rId5"/>
+    <sheet name="AltaMasiva" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="65">
   <si>
     <t>Descripción</t>
   </si>
@@ -125,13 +126,106 @@
   </si>
   <si>
     <t>Cuenta Bolsa</t>
+  </si>
+  <si>
+    <t>Alta de Linea</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>Provincia</t>
+  </si>
+  <si>
+    <t>Plan con Tarjeta Repro </t>
+  </si>
+  <si>
+    <t>IVA Consumidor Final</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Plan Prepago Nacional</t>
+  </si>
+  <si>
+    <t>CABA</t>
+  </si>
+  <si>
+    <t>Chaco</t>
+  </si>
+  <si>
+    <t>Chubut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Córdoba </t>
+  </si>
+  <si>
+    <t>Corrientes</t>
+  </si>
+  <si>
+    <t>Entre Ríos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formosa </t>
+  </si>
+  <si>
+    <t>Jujuy</t>
+  </si>
+  <si>
+    <t>La Rioja</t>
+  </si>
+  <si>
+    <t>Mendoza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Misiones </t>
+  </si>
+  <si>
+    <t>Neuquén</t>
+  </si>
+  <si>
+    <t>Rio Negro</t>
+  </si>
+  <si>
+    <t>Salta</t>
+  </si>
+  <si>
+    <t>San Juan</t>
+  </si>
+  <si>
+    <t>Santa Cruz</t>
+  </si>
+  <si>
+    <t>Santa Fe</t>
+  </si>
+  <si>
+    <t>Sgo. Del Estero</t>
+  </si>
+  <si>
+    <t>Tierra del Fuego</t>
+  </si>
+  <si>
+    <t>Tucumán</t>
+  </si>
+  <si>
+    <t>Catamarca</t>
+  </si>
+  <si>
+    <t>La Pampa</t>
+  </si>
+  <si>
+    <t>San Luis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -155,8 +249,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,8 +268,20 @@
         <bgColor rgb="FFF3715A"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD99594"/>
+        <bgColor rgb="FFD99594"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8CCE4"/>
+        <bgColor rgb="FFB8CCE4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -207,11 +318,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -231,9 +358,12 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -518,16 +648,16 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -563,7 +693,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -573,7 +703,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -583,7 +713,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -593,7 +723,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -615,20 +745,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +794,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -678,7 +808,7 @@
         <v>1160444719</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -692,7 +822,7 @@
         <v>1157572274</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
@@ -704,7 +834,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -715,7 +845,7 @@
         <v>22355504</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -744,16 +874,16 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,7 +919,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -817,17 +947,17 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,7 +993,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -893,16 +1023,16 @@
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="13" width="11.5546875" customWidth="1"/>
-    <col min="14" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,7 +1066,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -955,4 +1085,407 @@
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+    </row>
+    <row r="2" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test de Perfoman, Befan y actualizacion
Se agrega el paquete Perfomance para los caos, se agrega la clase de login para el perfomance.

Se Agerga la Page BeFAN incompleta.
Se agrega Test Befan Incompleto.

Se agrega la Hoja login con los datos de logueo en el archivo login
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -5,25 +5,26 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\telecom2\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14208" windowHeight="1620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
     <sheet name="Sales" sheetId="2" r:id="rId2"/>
-    <sheet name="Customer" sheetId="3" r:id="rId3"/>
-    <sheet name="Tech" sheetId="4" r:id="rId4"/>
-    <sheet name="SCP" sheetId="5" r:id="rId5"/>
+    <sheet name="Login" sheetId="6" r:id="rId3"/>
+    <sheet name="Customer" sheetId="3" r:id="rId4"/>
+    <sheet name="Tech" sheetId="4" r:id="rId5"/>
+    <sheet name="SCP" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Descripción</t>
   </si>
@@ -131,13 +132,58 @@
   </si>
   <si>
     <t>Pasaporte Bolsa</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Contraseña</t>
+  </si>
+  <si>
+    <t>Ambiente</t>
+  </si>
+  <si>
+    <t>Tiempo(S)</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>u589831</t>
+  </si>
+  <si>
+    <t>Testa10k</t>
+  </si>
+  <si>
+    <t>CRM</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>u198427</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>u590422</t>
+  </si>
+  <si>
+    <t>u580714</t>
+  </si>
+  <si>
+    <t>u581441</t>
+  </si>
+  <si>
+    <t>https://crm--sit.cs14.my.salesforce.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -161,8 +207,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4" tint="0.79998168889431442"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +231,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF3715A"/>
         <bgColor rgb="FFF3715A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -217,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,6 +301,9 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,16 +591,16 @@
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,7 +636,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -579,7 +646,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -589,7 +656,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -599,7 +666,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -621,20 +688,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +737,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -684,7 +751,7 @@
         <v>1160444719</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -698,7 +765,7 @@
         <v>1157572274</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
@@ -710,7 +777,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -721,7 +788,7 @@
         <v>22355504</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -735,7 +802,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -761,22 +828,145 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="14">
+        <v>15</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="14">
+        <v>15</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="14">
+        <v>15</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="14">
+        <v>15</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -812,7 +1002,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -832,7 +1022,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -840,17 +1030,17 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,7 +1076,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -908,7 +1098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -916,16 +1106,16 @@
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="13" width="11.5546875" customWidth="1"/>
-    <col min="14" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +1149,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Cambio en Archivo para test de Perfomance
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -869,7 +869,7 @@
         <v>42</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>50</v>
@@ -886,7 +886,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="14">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>50</v>
@@ -903,7 +903,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="14">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>50</v>
@@ -920,7 +920,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="14">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>50</v>
@@ -937,7 +937,7 @@
         <v>42</v>
       </c>
       <c r="D6" s="14">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
2018-05-03 - Update BasePage & Create Marketing & Create Marketing_Mattu
BasePage
   Update selectMainTabByName()

Marketing
   Create goToAccountTab()

Marketing_Mattu
   TS98035_Label_TyC_Alta_CP()
   TS98034_Link_TyC_Alta_CP()
   TS90288_Eliminaci�n_de_Campo_Segmento_Segment_C()
   Update several Priorities
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\telecom2\TelecomProyectoFAN\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="2"/>
+    <workbookView xWindow="945" yWindow="0" windowWidth="18765" windowHeight="6645"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -20,11 +15,12 @@
     <sheet name="SCP" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:J20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Descripción</t>
   </si>
@@ -177,13 +173,19 @@
   </si>
   <si>
     <t>https://crm--sit.cs14.my.salesforce.com/</t>
+  </si>
+  <si>
+    <t>Cuenta Atributos y Exclusiones</t>
+  </si>
+  <si>
+    <t>aaaaCuenta Marketing AYC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -216,6 +218,19 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -281,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,6 +319,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,11 +601,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -674,9 +691,20 @@
         <v>29</v>
       </c>
     </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="16"/>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -830,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cambios OM y Sales
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\telecom2\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florangel\git\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="Customer" sheetId="3" r:id="rId4"/>
     <sheet name="Tech" sheetId="4" r:id="rId5"/>
     <sheet name="SCP" sheetId="5" r:id="rId6"/>
+    <sheet name="OM" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="118">
   <si>
     <t>Descripción</t>
   </si>
@@ -177,13 +178,214 @@
   </si>
   <si>
     <t>https://crm--sit.cs14.my.salesforce.com/</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>ICCID</t>
+  </si>
+  <si>
+    <t>IMSI</t>
+  </si>
+  <si>
+    <t>KI</t>
+  </si>
+  <si>
+    <t>5C049A9A641145830238E32A56209EE4</t>
+  </si>
+  <si>
+    <t>897CEE307629B136627BC7324A10ECBE</t>
+  </si>
+  <si>
+    <t>1ADFCB2A332ED5212989D20DEA831F6B</t>
+  </si>
+  <si>
+    <t>E88C903A5A040AD8E67FB1C6DD0CEB08</t>
+  </si>
+  <si>
+    <t>4F858B01D23CD6CEBB81B0E5D35FBC54</t>
+  </si>
+  <si>
+    <t>4DEE8B9FA961BCAA9CCE1F54E0B4FB5D</t>
+  </si>
+  <si>
+    <t>33300BE31FEB8727D972F3FDD0FA81D8</t>
+  </si>
+  <si>
+    <t>8BF3BEA360425B7FBE2AF512B77BA445</t>
+  </si>
+  <si>
+    <t>D744410171750B43350230DA526B45CA</t>
+  </si>
+  <si>
+    <t>FF257DF0339972FBDFDDE492EDA2869A</t>
+  </si>
+  <si>
+    <t>A82D1595C7326E6D318E8D59D828A518</t>
+  </si>
+  <si>
+    <t>70504AE10E305C9AE08449C20FC83C0C</t>
+  </si>
+  <si>
+    <t>B8A875F61A823A308385FAF29C52EB81</t>
+  </si>
+  <si>
+    <t>FFE374222C8BEEAF149517B1D9BF487A</t>
+  </si>
+  <si>
+    <t>460BDBE305E0BB63D28A42795CED52D7</t>
+  </si>
+  <si>
+    <t>15D5D387805FE2759759DFBEA7FDF1F1</t>
+  </si>
+  <si>
+    <t>75B8775BD64FC6C48C83FDC14FF8D640</t>
+  </si>
+  <si>
+    <t>6F7004355C60CDB0BC5A25CD97DB3D88</t>
+  </si>
+  <si>
+    <t>F8F53FA426AA7CE9AECAC3E9747E0F64</t>
+  </si>
+  <si>
+    <t>0F8AC89E9EEAC900E9DBB9E3EE9712DA</t>
+  </si>
+  <si>
+    <t>Plan Prepago Nacional</t>
+  </si>
+  <si>
+    <t>Plan con Tarjeta</t>
+  </si>
+  <si>
+    <t>Victor Rodriguez</t>
+  </si>
+  <si>
+    <t>AltaLinea</t>
+  </si>
+  <si>
+    <t>Alta Linea</t>
+  </si>
+  <si>
+    <t>89543410707701993310</t>
+  </si>
+  <si>
+    <t>89543410707701993328</t>
+  </si>
+  <si>
+    <t>89543410707701993336</t>
+  </si>
+  <si>
+    <t>89543410707701993344</t>
+  </si>
+  <si>
+    <t>89543410707701993351</t>
+  </si>
+  <si>
+    <t>89543410707701993369</t>
+  </si>
+  <si>
+    <t>89543410707701993377</t>
+  </si>
+  <si>
+    <t>89543410707701993385</t>
+  </si>
+  <si>
+    <t>89543410707701993393</t>
+  </si>
+  <si>
+    <t>89543410707701993401</t>
+  </si>
+  <si>
+    <t>89543410707701993419</t>
+  </si>
+  <si>
+    <t>89543410707701993427</t>
+  </si>
+  <si>
+    <t>89543410707701993435</t>
+  </si>
+  <si>
+    <t>89543410707701993443</t>
+  </si>
+  <si>
+    <t>89543410707701993450</t>
+  </si>
+  <si>
+    <t>89543410707701993468</t>
+  </si>
+  <si>
+    <t>89543410707701993476</t>
+  </si>
+  <si>
+    <t>89543410707701993484</t>
+  </si>
+  <si>
+    <t>89543410707701993492</t>
+  </si>
+  <si>
+    <t>89543410707701993500</t>
+  </si>
+  <si>
+    <t>CambioSim</t>
+  </si>
+  <si>
+    <t>Nuevo ICCID</t>
+  </si>
+  <si>
+    <t>Nuevo IMSI</t>
+  </si>
+  <si>
+    <t>Nuevo KI</t>
+  </si>
+  <si>
+    <t>83AB7B84FB724C7085AD97B82B692250</t>
+  </si>
+  <si>
+    <t>89543410707701993518</t>
+  </si>
+  <si>
+    <t>89543410707701993526</t>
+  </si>
+  <si>
+    <t>F21711F8F90D1A10A431AC57399B2EDA</t>
+  </si>
+  <si>
+    <t>89543410707701993534</t>
+  </si>
+  <si>
+    <t>89543410707701993542</t>
+  </si>
+  <si>
+    <t>2D0B71CFF76434465392B0448B7B5340</t>
+  </si>
+  <si>
+    <t>DC1304020BFD01F2A48C9BFD0EF9DEA3</t>
+  </si>
+  <si>
+    <t>Cambio Sim</t>
+  </si>
+  <si>
+    <t>89543410707701993559</t>
+  </si>
+  <si>
+    <t>89543410707701993567</t>
+  </si>
+  <si>
+    <t>4F2120C5131167B9D109F21EF2147CAC</t>
+  </si>
+  <si>
+    <t>251AD9F138DD4030A5349E60693FD32E</t>
+  </si>
+  <si>
+    <t>Nominacion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -219,8 +421,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,8 +447,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -277,11 +491,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,6 +542,18 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,7 +939,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -830,7 +1080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
@@ -1168,4 +1418,664 @@
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="40.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="17">
+        <v>3413104291</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="18">
+        <v>722341170199331</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="17">
+        <v>3413104292</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="18">
+        <v>722341170199332</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="17">
+        <v>3413104293</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="18">
+        <v>722341170199333</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="17">
+        <v>3413104294</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="18">
+        <v>722341170199334</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" s="17">
+        <v>3413104295</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="18">
+        <v>722341170199335</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="17">
+        <v>3413104296</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="18">
+        <v>722341170199336</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D8" s="17">
+        <v>3413104297</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="18">
+        <v>722341170199337</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="17">
+        <v>3413104298</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="18">
+        <v>722341170199338</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="17">
+        <v>3413104299</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="18">
+        <v>722341170199339</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D11" s="17">
+        <v>3413104300</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="18">
+        <v>722341170199340</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="17">
+        <v>3413104301</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="18">
+        <v>722341170199341</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="17">
+        <v>3413104302</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="18">
+        <v>722341170199342</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="17">
+        <v>3413104303</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="18">
+        <v>722341170199343</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="17">
+        <v>3413104304</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="18">
+        <v>722341170199344</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="17">
+        <v>3413104305</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="18">
+        <v>722341170199345</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="17">
+        <v>3413104306</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="18">
+        <v>722341170199346</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="17">
+        <v>3413104307</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="18">
+        <v>722341170199347</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="17">
+        <v>3413104308</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="18">
+        <v>722341170199348</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D20" s="17">
+        <v>3413104309</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="18">
+        <v>722341170199349</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="17">
+        <v>3413104310</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="18">
+        <v>722341170199350</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="14">
+        <v>3413104311</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="18">
+        <v>722341170199351</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="I22" s="18">
+        <v>722341170199353</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="14">
+        <v>3413104312</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="18">
+        <v>722341170199352</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="I23" s="18">
+        <v>722341170199354</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="14">
+        <v>3413104313</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="18">
+        <v>722341170199355</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="14">
+        <v>3413104314</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="18">
+        <v>722341170199356</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26">
+        <v>10000018</v>
+      </c>
+      <c r="D26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en todo 3-7-18
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -378,9 +378,6 @@
     <t>251AD9F138DD4030A5349E60693FD32E</t>
   </si>
   <si>
-    <t>Nomina cion</t>
-  </si>
-  <si>
     <t>Victorchichito Rodriguez</t>
   </si>
   <si>
@@ -826,6 +823,9 @@
   </si>
   <si>
     <t>CambioDeNumero</t>
+  </si>
+  <si>
+    <t>Nominacion</t>
   </si>
 </sst>
 </file>
@@ -1898,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2536,7 +2536,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>117</v>
+        <v>266</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>32</v>
@@ -2553,22 +2553,22 @@
         <v>78</v>
       </c>
       <c r="B27" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="D27" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2576,22 +2576,22 @@
         <v>78</v>
       </c>
       <c r="B28" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D28" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="F28" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="G28" s="20" t="s">
         <v>126</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2599,22 +2599,22 @@
         <v>78</v>
       </c>
       <c r="B29" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D29" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="F29" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2622,22 +2622,22 @@
         <v>78</v>
       </c>
       <c r="B30" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D30" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="F30" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="G30" s="20" t="s">
         <v>134</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2645,22 +2645,22 @@
         <v>78</v>
       </c>
       <c r="B31" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D31" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="F31" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="G31" s="20" t="s">
         <v>138</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2668,22 +2668,22 @@
         <v>78</v>
       </c>
       <c r="B32" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D32" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="F32" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="G32" s="20" t="s">
         <v>142</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2691,22 +2691,22 @@
         <v>78</v>
       </c>
       <c r="B33" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D33" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="F33" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="G33" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2714,22 +2714,22 @@
         <v>78</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D34" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="F34" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="G34" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2737,22 +2737,22 @@
         <v>78</v>
       </c>
       <c r="B35" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D35" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="F35" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2760,22 +2760,22 @@
         <v>78</v>
       </c>
       <c r="B36" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>119</v>
-      </c>
       <c r="D36" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="F36" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>158</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2783,22 +2783,22 @@
         <v>78</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="E37" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="F37" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>163</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2806,22 +2806,22 @@
         <v>78</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D38" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="F38" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>167</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2829,22 +2829,22 @@
         <v>78</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D39" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="F39" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>171</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2852,22 +2852,22 @@
         <v>78</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D40" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="F40" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="G40" s="20" t="s">
         <v>175</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2875,22 +2875,22 @@
         <v>78</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D41" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="F41" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="G41" s="20" t="s">
         <v>179</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2898,22 +2898,22 @@
         <v>78</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D42" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E42" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="F42" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="G42" s="20" t="s">
         <v>183</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2921,22 +2921,22 @@
         <v>78</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D43" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="F43" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="G43" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2944,22 +2944,22 @@
         <v>78</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D44" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="F44" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="G44" s="20" t="s">
         <v>191</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2967,22 +2967,22 @@
         <v>78</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D45" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="E45" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="F45" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="G45" s="20" t="s">
         <v>195</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -2990,22 +2990,22 @@
         <v>78</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D46" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="E46" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="F46" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="G46" s="20" t="s">
         <v>199</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -3013,31 +3013,31 @@
         <v>100</v>
       </c>
       <c r="B47" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C47" s="21" t="s">
-        <v>119</v>
-      </c>
       <c r="D47" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="E47" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="F47" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="G47" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="H47" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="I47" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="I47" s="21" t="s">
+      <c r="J47" s="21" t="s">
         <v>206</v>
-      </c>
-      <c r="J47" s="21" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -3045,246 +3045,246 @@
         <v>100</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D48" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="E48" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="F48" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="G48" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="H48" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="I48" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="I48" s="21" t="s">
+      <c r="J48" s="21" t="s">
         <v>213</v>
-      </c>
-      <c r="J48" s="21" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B49" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C49" s="21" t="s">
-        <v>119</v>
-      </c>
       <c r="D49" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="E49" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="F49" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="G49" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="H49" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="H49" s="21" t="s">
+      <c r="I49" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="I49" s="21" t="s">
+      <c r="J49" s="21" t="s">
         <v>220</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B50" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>119</v>
-      </c>
       <c r="D50" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="E50" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="F50" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="G50" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="H50" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="I50" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="I50" s="21" t="s">
+      <c r="J50" s="21" t="s">
         <v>227</v>
-      </c>
-      <c r="J50" s="21" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B51" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C51" s="21" t="s">
-        <v>119</v>
-      </c>
       <c r="D51" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="E51" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="F51" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="G51" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="H51" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="I51" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="I51" s="21" t="s">
+      <c r="J51" s="21" t="s">
         <v>234</v>
-      </c>
-      <c r="J51" s="21" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D52" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="E52" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="F52" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="G52" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="H52" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="H52" s="21" t="s">
+      <c r="I52" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="I52" s="21" t="s">
+      <c r="J52" s="21" t="s">
         <v>241</v>
-      </c>
-      <c r="J52" s="21" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D53" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="E53" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="F53" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="G53" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="H53" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="H53" s="21" t="s">
+      <c r="I53" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="I53" s="21" t="s">
+      <c r="J53" s="21" t="s">
         <v>248</v>
-      </c>
-      <c r="J53" s="21" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D54" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="E54" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="F54" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="G54" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="H54" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="H54" s="21" t="s">
+      <c r="I54" s="21" t="s">
         <v>254</v>
       </c>
-      <c r="I54" s="21" t="s">
+      <c r="J54" s="21" t="s">
         <v>255</v>
-      </c>
-      <c r="J54" s="21" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B55" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>119</v>
-      </c>
       <c r="D55" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>258</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="F55" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="G55" s="22" t="s">
         <v>260</v>
-      </c>
-      <c r="G55" s="22" t="s">
-        <v>261</v>
       </c>
       <c r="H55">
         <v>2514856214</v>
@@ -3292,25 +3292,25 @@
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D56" s="22" t="s">
+        <v>261</v>
+      </c>
+      <c r="E56" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="F56" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="F56" s="22" t="s">
+      <c r="G56" s="22" t="s">
         <v>264</v>
-      </c>
-      <c r="G56" s="22" t="s">
-        <v>265</v>
       </c>
       <c r="H56">
         <v>2548965321</v>

</xml_diff>

<commit_message>
todo cambio por perfiles nuevos
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="269">
   <si>
     <t>Descripción</t>
   </si>
@@ -327,9 +327,6 @@
     <t>89543410707701993500</t>
   </si>
   <si>
-    <t>CambioSim</t>
-  </si>
-  <si>
     <t>Nuevo ICCID</t>
   </si>
   <si>
@@ -795,9 +792,6 @@
     <t>2AE90F17B3259C179331C48A6CFC5506</t>
   </si>
   <si>
-    <t>CambioSimSiniestro</t>
-  </si>
-  <si>
     <t>3413104357</t>
   </si>
   <si>
@@ -822,21 +816,40 @@
     <t>610C18706E4A00E42436647ADF9996A4</t>
   </si>
   <si>
-    <t>CambioDeNumero</t>
-  </si>
-  <si>
     <t>Nominacion</t>
+  </si>
+  <si>
+    <t>Cambio SimSiniestro</t>
+  </si>
+  <si>
+    <t>Cambio DeNumero</t>
+  </si>
+  <si>
+    <t>FlorOM</t>
+  </si>
+  <si>
+    <t>E76E60CD50</t>
+  </si>
+  <si>
+    <t>todo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -908,7 +921,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -984,49 +997,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1896,10 +1920,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z56"/>
+  <dimension ref="A1:Z57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1939,13 +1963,13 @@
         <v>54</v>
       </c>
       <c r="H1" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -2426,7 +2450,7 @@
     </row>
     <row r="22" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>77</v>
@@ -2438,27 +2462,27 @@
         <v>3413104311</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F22" s="18">
         <v>722341170199351</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I22" s="18">
         <v>722341170199353</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>77</v>
@@ -2470,22 +2494,22 @@
         <v>3413104312</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F23" s="18">
         <v>722341170199352</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I23" s="18">
         <v>722341170199354</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2502,13 +2526,13 @@
         <v>3413104313</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F24" s="18">
         <v>722341170199355</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -2525,18 +2549,18 @@
         <v>3413104314</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F25" s="18">
         <v>722341170199356</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>32</v>
@@ -2550,718 +2574,718 @@
     </row>
     <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B27" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="D27" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>121</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B28" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D28" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="F28" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="G28" s="20" t="s">
         <v>125</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B29" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D29" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="F29" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>129</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B30" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D30" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="F30" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="G30" s="20" t="s">
         <v>133</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B31" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D31" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="E31" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="F31" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="G31" s="20" t="s">
         <v>137</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B32" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D32" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="E32" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="F32" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="G32" s="20" t="s">
         <v>141</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B33" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D33" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="F33" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="G33" s="20" t="s">
         <v>145</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D34" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E34" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="F34" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="G34" s="20" t="s">
         <v>149</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B35" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D35" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="F35" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>153</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>118</v>
-      </c>
       <c r="D36" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="E36" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="F36" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>157</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C37" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="E37" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="F37" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>162</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D38" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="F38" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>166</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D39" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="F39" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>170</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D40" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="E40" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="F40" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="G40" s="20" t="s">
         <v>174</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D41" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="E41" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="F41" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="G41" s="20" t="s">
         <v>178</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D42" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E42" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="F42" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="G42" s="20" t="s">
         <v>182</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D43" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="F43" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="G43" s="20" t="s">
         <v>186</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D44" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="E44" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="F44" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="G44" s="20" t="s">
         <v>190</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D45" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="E45" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="F45" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="G45" s="20" t="s">
         <v>194</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D46" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="E46" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="F46" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="G46" s="20" t="s">
         <v>198</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B47" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C47" s="21" t="s">
-        <v>118</v>
-      </c>
       <c r="D47" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="E47" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="F47" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="G47" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="H47" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="I47" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="I47" s="21" t="s">
+      <c r="J47" s="21" t="s">
         <v>205</v>
-      </c>
-      <c r="J47" s="21" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D48" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="E48" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="F48" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="G48" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="H48" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="I48" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="I48" s="21" t="s">
+      <c r="J48" s="21" t="s">
         <v>212</v>
-      </c>
-      <c r="J48" s="21" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B49" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="21" t="s">
-        <v>118</v>
-      </c>
       <c r="D49" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="E49" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="F49" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="G49" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="H49" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="H49" s="21" t="s">
+      <c r="I49" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="I49" s="21" t="s">
+      <c r="J49" s="21" t="s">
         <v>219</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B50" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C50" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>118</v>
-      </c>
       <c r="D50" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="E50" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="F50" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="G50" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="H50" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="I50" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="I50" s="21" t="s">
+      <c r="J50" s="21" t="s">
         <v>226</v>
-      </c>
-      <c r="J50" s="21" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B51" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C51" s="21" t="s">
-        <v>118</v>
-      </c>
       <c r="D51" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="E51" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="F51" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="G51" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="H51" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="I51" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="I51" s="21" t="s">
+      <c r="J51" s="21" t="s">
         <v>233</v>
-      </c>
-      <c r="J51" s="21" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D52" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="E52" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="F52" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="G52" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="H52" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="H52" s="21" t="s">
+      <c r="I52" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="I52" s="21" t="s">
+      <c r="J52" s="21" t="s">
         <v>240</v>
-      </c>
-      <c r="J52" s="21" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D53" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="E53" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="F53" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="G53" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="H53" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="H53" s="21" t="s">
+      <c r="I53" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="I53" s="21" t="s">
+      <c r="J53" s="21" t="s">
         <v>247</v>
-      </c>
-      <c r="J53" s="21" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D54" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="E54" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="F54" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="G54" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="H54" s="21" t="s">
         <v>252</v>
       </c>
-      <c r="H54" s="21" t="s">
+      <c r="I54" s="21" t="s">
         <v>253</v>
       </c>
-      <c r="I54" s="21" t="s">
+      <c r="J54" s="21" t="s">
         <v>254</v>
-      </c>
-      <c r="J54" s="21" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -3269,22 +3293,22 @@
         <v>265</v>
       </c>
       <c r="B55" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>118</v>
-      </c>
       <c r="D55" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="F55" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="G55" s="22" t="s">
         <v>258</v>
-      </c>
-      <c r="F55" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="G55" s="22" t="s">
-        <v>260</v>
       </c>
       <c r="H55">
         <v>2514856214</v>
@@ -3295,25 +3319,51 @@
         <v>265</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D56" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>260</v>
+      </c>
+      <c r="F56" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="G56" s="22" t="s">
         <v>262</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="G56" s="22" t="s">
-        <v>264</v>
       </c>
       <c r="H56">
         <v>2548965321</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="22">
+        <v>2213104354</v>
+      </c>
+      <c r="E57" s="22">
+        <v>895434</v>
+      </c>
+      <c r="F57" s="22">
+        <v>72234</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="H57" s="24" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OM y Sales 20/07/2018
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
     <sheet name="Sales" sheetId="2" r:id="rId2"/>
-    <sheet name="Login" sheetId="6" r:id="rId3"/>
-    <sheet name="Customer" sheetId="3" r:id="rId4"/>
-    <sheet name="Tech" sheetId="4" r:id="rId5"/>
-    <sheet name="SCP" sheetId="5" r:id="rId6"/>
-    <sheet name="OM" sheetId="7" r:id="rId7"/>
+    <sheet name="PreparacionDatos" sheetId="8" r:id="rId3"/>
+    <sheet name="Login" sheetId="6" r:id="rId4"/>
+    <sheet name="Customer" sheetId="3" r:id="rId5"/>
+    <sheet name="Tech" sheetId="4" r:id="rId6"/>
+    <sheet name="SCP" sheetId="5" r:id="rId7"/>
+    <sheet name="OM" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="283">
   <si>
     <t>Descripción</t>
   </si>
@@ -841,13 +842,46 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>Fecha Nacimiento</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Malan</t>
+  </si>
+  <si>
+    <t>Fareto</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>malannominacion@gmail.com</t>
+  </si>
+  <si>
+    <t>08/08/1992</t>
+  </si>
+  <si>
+    <t>543416748666</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -909,6 +943,12 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1036,11 +1076,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1085,8 +1126,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1471,7 +1516,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1610,6 +1655,108 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="5" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2">
+        <v>52486595</v>
+      </c>
+      <c r="E2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2" t="s">
+        <v>278</v>
+      </c>
+      <c r="G2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1731,7 +1878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1804,7 +1951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1880,7 +2027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1952,11 +2099,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
+    <sheetView topLeftCell="E43" workbookViewId="0">
       <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
cambios en todo 26-7
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14205" windowHeight="1620" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="SCP" sheetId="5" r:id="rId7"/>
     <sheet name="OM" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="294">
   <si>
     <t>Descripción</t>
   </si>
@@ -874,7 +874,40 @@
     <t>08/08/1992</t>
   </si>
   <si>
-    <t>543416748666</t>
+    <t>543416876777</t>
+  </si>
+  <si>
+    <t>vicente lopez</t>
+  </si>
+  <si>
+    <t>Buenos Aires</t>
+  </si>
+  <si>
+    <t>Provincia</t>
+  </si>
+  <si>
+    <t>Localidad</t>
+  </si>
+  <si>
+    <t>Linea</t>
+  </si>
+  <si>
+    <t>52648975215</t>
+  </si>
+  <si>
+    <t>15425684</t>
+  </si>
+  <si>
+    <t>25489645</t>
+  </si>
+  <si>
+    <t>14756841</t>
+  </si>
+  <si>
+    <t>Natias</t>
+  </si>
+  <si>
+    <t>Mazano</t>
   </si>
 </sst>
 </file>
@@ -1655,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1667,6 +1700,8 @@
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.140625" customWidth="1"/>
     <col min="4" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
   </cols>
@@ -1675,35 +1710,45 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>3</v>
+        <v>272</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>273</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>275</v>
+        <v>51</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+        <v>285</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
@@ -1719,39 +1764,129 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="32">
+        <v>59885659</v>
+      </c>
+      <c r="C2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E2" t="s">
+        <v>279</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="H2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" t="s">
+        <v>284</v>
+      </c>
+      <c r="J2" t="s">
+        <v>283</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="32">
+        <v>59885660</v>
+      </c>
+      <c r="C3" t="s">
+        <v>292</v>
+      </c>
+      <c r="D3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" t="s">
+        <v>279</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="H3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" t="s">
+        <v>284</v>
+      </c>
+      <c r="J3" t="s">
+        <v>283</v>
+      </c>
+      <c r="K3" s="32" t="s">
+        <v>288</v>
+      </c>
+      <c r="L3" s="32" t="s">
+        <v>289</v>
+      </c>
+      <c r="M3" s="32" t="s">
+        <v>290</v>
+      </c>
+      <c r="N3" s="32" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>263</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C4" s="32" t="s">
         <v>282</v>
       </c>
-      <c r="D2">
+      <c r="D4">
         <v>52486595</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E4" t="s">
         <v>277</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F4" t="s">
         <v>278</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G4" t="s">
         <v>279</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H4" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I4" s="30" t="s">
         <v>280</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="I4" r:id="rId2"/>
+    <hyperlink ref="G3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2103,8 +2238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z58"/>
   <sheetViews>
-    <sheetView topLeftCell="E43" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Todo cambio v v 1-8-18
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="300">
   <si>
     <t>Descripción</t>
   </si>
@@ -892,28 +892,40 @@
     <t>Linea</t>
   </si>
   <si>
-    <t>52648975215</t>
-  </si>
-  <si>
-    <t>15425684</t>
-  </si>
-  <si>
-    <t>25489645</t>
-  </si>
-  <si>
-    <t>14756841</t>
-  </si>
-  <si>
     <t>Natias</t>
   </si>
   <si>
     <t>Mazano</t>
   </si>
   <si>
-    <t>59885661</t>
-  </si>
-  <si>
-    <t>59885662</t>
+    <t>Numeros Amigos</t>
+  </si>
+  <si>
+    <t>Ruben</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>27/08/1987</t>
+  </si>
+  <si>
+    <t>rubenrod@gmail.com</t>
+  </si>
+  <si>
+    <t>1185946824</t>
+  </si>
+  <si>
+    <t>59885673</t>
+  </si>
+  <si>
+    <t>59885702</t>
+  </si>
+  <si>
+    <t>Alta Linea Agente</t>
+  </si>
+  <si>
+    <t>59885103</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1567,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1694,10 +1706,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1770,10 +1782,10 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>298</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="C2" t="s">
         <v>277</v>
@@ -1799,31 +1811,23 @@
       <c r="J2" t="s">
         <v>283</v>
       </c>
-      <c r="K2" s="32" t="s">
-        <v>288</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>290</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>291</v>
-      </c>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E3" t="s">
         <v>279</v>
@@ -1843,18 +1847,10 @@
       <c r="J3" t="s">
         <v>283</v>
       </c>
-      <c r="K3" s="32" t="s">
-        <v>288</v>
-      </c>
-      <c r="L3" s="32" t="s">
-        <v>289</v>
-      </c>
-      <c r="M3" s="32" t="s">
-        <v>290</v>
-      </c>
-      <c r="N3" s="32" t="s">
-        <v>291</v>
-      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1884,15 +1880,56 @@
       <c r="I4" s="30" t="s">
         <v>280</v>
       </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>296</v>
+      </c>
+      <c r="C5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D5" t="s">
+        <v>292</v>
+      </c>
+      <c r="E5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>293</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>294</v>
+      </c>
+      <c r="H5" t="s">
+        <v>158</v>
+      </c>
+      <c r="I5" t="s">
+        <v>284</v>
+      </c>
+      <c r="J5" t="s">
+        <v>283</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>295</v>
+      </c>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="I4" r:id="rId2"/>
     <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="G5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1901,7 +1938,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
2018-08-03 - Create Cuentas & Create TestBase & Fix GestionesPerfilOfici
Create Sheet PerfilGestiones on Cuentas
Create DataProviders PerfilCuentaSeiscientos() & PerfilCuentaTomRiddle() on TestBase
Update @dataProvider on GestionesPerfilOficina
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14208" windowHeight="1620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -20,13 +15,15 @@
     <sheet name="Tech" sheetId="4" r:id="rId6"/>
     <sheet name="SCP" sheetId="5" r:id="rId7"/>
     <sheet name="OM" sheetId="7" r:id="rId8"/>
+    <sheet name="NumeroAmigo" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:H42"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="309">
   <si>
     <t>Descripción</t>
   </si>
@@ -938,6 +935,21 @@
   </si>
   <si>
     <t>Nicetto@gmail.com</t>
+  </si>
+  <si>
+    <t>Titular de producto/servicio</t>
+  </si>
+  <si>
+    <t>Cuenta Seiscientos</t>
+  </si>
+  <si>
+    <t>Numero de Cuenta</t>
+  </si>
+  <si>
+    <t>9900000698210001</t>
+  </si>
+  <si>
+    <t>Línea</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1156,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1193,6 +1205,14 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1478,20 +1498,20 @@
   <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +1547,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1537,7 +1557,7 @@
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1547,7 +1567,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1557,7 +1577,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1580,19 +1600,19 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1628,7 +1648,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1642,7 +1662,7 @@
         <v>1160444719</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1656,7 +1676,7 @@
         <v>1157572274</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
@@ -1668,7 +1688,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1679,7 +1699,7 @@
         <v>22355504</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1693,7 +1713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -1721,23 +1741,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1793,7 +1813,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>298</v>
       </c>
@@ -1829,7 +1849,7 @@
       <c r="M2" s="32"/>
       <c r="N2" s="32"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1865,7 +1885,7 @@
       <c r="M3" s="32"/>
       <c r="N3" s="32"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>263</v>
       </c>
@@ -1894,7 +1914,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -1934,7 +1954,7 @@
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>300</v>
       </c>
@@ -1984,17 +2004,17 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>40</v>
       </c>
@@ -2011,7 +2031,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>43</v>
       </c>
@@ -2028,7 +2048,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>44</v>
       </c>
@@ -2045,7 +2065,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
@@ -2062,7 +2082,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>46</v>
       </c>
@@ -2079,7 +2099,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>46</v>
       </c>
@@ -2107,19 +2127,19 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2155,7 +2175,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2180,20 +2200,20 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2229,7 +2249,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -2259,16 +2279,16 @@
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="13" width="11.5546875" customWidth="1"/>
-    <col min="14" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2322,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -2328,24 +2348,24 @@
   <dimension ref="A1:Z58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
-    <col min="7" max="7" width="38.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2393,7 +2413,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>79</v>
       </c>
@@ -2416,7 +2436,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>79</v>
       </c>
@@ -2439,7 +2459,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>79</v>
       </c>
@@ -2462,7 +2482,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>79</v>
       </c>
@@ -2485,7 +2505,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>79</v>
       </c>
@@ -2508,7 +2528,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>79</v>
       </c>
@@ -2531,7 +2551,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>79</v>
       </c>
@@ -2554,7 +2574,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>79</v>
       </c>
@@ -2577,7 +2597,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>79</v>
       </c>
@@ -2600,7 +2620,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>79</v>
       </c>
@@ -2623,7 +2643,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>79</v>
       </c>
@@ -2646,7 +2666,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>79</v>
       </c>
@@ -2669,7 +2689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>79</v>
       </c>
@@ -2692,7 +2712,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>79</v>
       </c>
@@ -2715,7 +2735,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>79</v>
       </c>
@@ -2738,7 +2758,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>79</v>
       </c>
@@ -2761,7 +2781,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>79</v>
       </c>
@@ -2784,7 +2804,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>79</v>
       </c>
@@ -2807,7 +2827,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>79</v>
       </c>
@@ -2830,7 +2850,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>79</v>
       </c>
@@ -2853,7 +2873,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>111</v>
       </c>
@@ -2885,7 +2905,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>111</v>
       </c>
@@ -2917,7 +2937,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>79</v>
       </c>
@@ -2940,7 +2960,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>79</v>
       </c>
@@ -2963,7 +2983,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -2977,7 +2997,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>79</v>
       </c>
@@ -3000,7 +3020,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>79</v>
       </c>
@@ -3023,7 +3043,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>79</v>
       </c>
@@ -3046,7 +3066,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>79</v>
       </c>
@@ -3069,7 +3089,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>79</v>
       </c>
@@ -3092,7 +3112,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>79</v>
       </c>
@@ -3115,7 +3135,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>79</v>
       </c>
@@ -3138,7 +3158,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>79</v>
       </c>
@@ -3161,7 +3181,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>79</v>
       </c>
@@ -3184,7 +3204,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>79</v>
       </c>
@@ -3207,7 +3227,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>79</v>
       </c>
@@ -3230,7 +3250,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>79</v>
       </c>
@@ -3253,7 +3273,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>79</v>
       </c>
@@ -3276,7 +3296,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>79</v>
       </c>
@@ -3299,7 +3319,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>79</v>
       </c>
@@ -3322,7 +3342,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>79</v>
       </c>
@@ -3345,7 +3365,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>79</v>
       </c>
@@ -3368,7 +3388,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>79</v>
       </c>
@@ -3391,7 +3411,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>79</v>
       </c>
@@ -3414,7 +3434,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>79</v>
       </c>
@@ -3437,7 +3457,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>111</v>
       </c>
@@ -3469,7 +3489,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>111</v>
       </c>
@@ -3501,7 +3521,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>264</v>
       </c>
@@ -3533,7 +3553,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>264</v>
       </c>
@@ -3565,7 +3585,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>264</v>
       </c>
@@ -3597,7 +3617,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>264</v>
       </c>
@@ -3629,7 +3649,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>264</v>
       </c>
@@ -3661,7 +3681,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>264</v>
       </c>
@@ -3693,7 +3713,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>265</v>
       </c>
@@ -3719,7 +3739,7 @@
         <v>2514856214</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>265</v>
       </c>
@@ -3745,7 +3765,7 @@
         <v>2548965321</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>78</v>
       </c>
@@ -3771,7 +3791,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>269</v>
       </c>
@@ -3806,6 +3826,93 @@
         <v>523654</v>
       </c>
     </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>306</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>308</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="39">
+        <v>46534534</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>307</v>
+      </c>
+      <c r="E2" s="5">
+        <v>1158423198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="34"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="35"/>
+    </row>
+    <row r="5" spans="1:27" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
alta linea cambio pak
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="337">
   <si>
     <t>Descripción</t>
   </si>
@@ -962,9 +962,6 @@
     <t>11/04/1989</t>
   </si>
   <si>
-    <t>59885779</t>
-  </si>
-  <si>
     <t>Recargas</t>
   </si>
   <si>
@@ -1019,12 +1016,6 @@
     <t>Ninguno</t>
   </si>
   <si>
-    <t>Steven Tyler</t>
-  </si>
-  <si>
-    <t>9900000718810001</t>
-  </si>
-  <si>
     <t>steventyler@gmail.com</t>
   </si>
   <si>
@@ -1035,6 +1026,18 @@
   </si>
   <si>
     <t>Venta de packs</t>
+  </si>
+  <si>
+    <t>59885788</t>
+  </si>
+  <si>
+    <t>Peter Quill</t>
+  </si>
+  <si>
+    <t>9900000687010001</t>
+  </si>
+  <si>
+    <t>Pack Internet x 30 dias</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1262,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1329,6 +1332,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1845,7 +1849,7 @@
     </row>
     <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B8" t="s">
         <v>277</v>
@@ -1869,7 +1873,7 @@
         <v>284</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="31"/>
@@ -1879,7 +1883,7 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B9" s="44">
         <v>46534534</v>
@@ -1894,7 +1898,7 @@
         <v>284</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -1905,7 +1909,7 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B10" s="44" t="s">
         <v>305</v>
@@ -1919,7 +1923,7 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="45" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B11" s="44" t="s">
         <v>309</v>
@@ -1949,7 +1953,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2166,7 +2170,7 @@
         <v>300</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>311</v>
+        <v>333</v>
       </c>
       <c r="C6" t="s">
         <v>301</v>
@@ -2195,10 +2199,10 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="B7" s="31" t="s">
         <v>324</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>325</v>
       </c>
       <c r="C7" t="s">
         <v>277</v>
@@ -2222,19 +2226,19 @@
         <v>284</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K7" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="L7" s="43" t="s">
         <v>326</v>
       </c>
-      <c r="L7" s="43" t="s">
+      <c r="M7" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="M7" s="31" t="s">
+      <c r="N7" s="31" t="s">
         <v>328</v>
-      </c>
-      <c r="N7" s="31" t="s">
-        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -4099,7 +4103,8 @@
     <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
+    <col min="7" max="14" width="11.5546875" customWidth="1"/>
     <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4193,7 +4198,7 @@
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B5" s="41">
         <v>23444455</v>
@@ -4202,19 +4207,19 @@
         <v>123</v>
       </c>
       <c r="D5" s="41" t="s">
+        <v>312</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="F5" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="G5" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="H5" s="31" t="s">
         <v>316</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>317</v>
       </c>
       <c r="I5" s="32">
         <v>4</v>
@@ -4226,7 +4231,7 @@
         <v>1234</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="M5" s="31">
         <v>19784521</v>
@@ -4238,53 +4243,56 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
-        <v>333</v>
-      </c>
-      <c r="B6" s="37">
-        <v>95000022</v>
+        <v>330</v>
+      </c>
+      <c r="B6" s="49">
+        <v>12543765</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="B7" s="49">
+        <v>12543765</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>334</v>
       </c>
-      <c r="B7" s="37">
-        <v>95000022</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>330</v>
-      </c>
       <c r="D7" s="47" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8" s="49">
+        <v>12543765</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>334</v>
+      </c>
+      <c r="D8" s="47" t="s">
         <v>335</v>
       </c>
-      <c r="B8" s="37">
-        <v>95000022</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>330</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>331</v>
-      </c>
       <c r="E8" s="48" t="s">
-        <v>332</v>
+        <v>329</v>
+      </c>
+      <c r="F8" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambios generales para regresion
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="348">
   <si>
     <t>Descripción</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Cuenta Activa c/Serv activo</t>
   </si>
   <si>
-    <t>aaaaFernando Care</t>
-  </si>
-  <si>
     <t>Cuenta Normal</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Cuenta Activa c/ linea y serv</t>
   </si>
   <si>
-    <t>Marco Polo</t>
-  </si>
-  <si>
     <t>Cuenta c/ oportunidades y prod</t>
   </si>
   <si>
@@ -926,9 +920,6 @@
     <t>Alta Linea Agente</t>
   </si>
   <si>
-    <t>59885103</t>
-  </si>
-  <si>
     <t>Alta Linea Equipo</t>
   </si>
   <si>
@@ -1050,6 +1041,36 @@
   </si>
   <si>
     <t>Ajustes</t>
+  </si>
+  <si>
+    <t>Santa Fe</t>
+  </si>
+  <si>
+    <t>Rosario</t>
+  </si>
+  <si>
+    <t>Falsa</t>
+  </si>
+  <si>
+    <t>1524</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosario </t>
+  </si>
+  <si>
+    <t>aaaaaMalan</t>
+  </si>
+  <si>
+    <t>59885133</t>
+  </si>
+  <si>
+    <t>59885136</t>
+  </si>
+  <si>
+    <t>AaaBbbMalan Fareto</t>
+  </si>
+  <si>
+    <t>3413105385</t>
   </si>
 </sst>
 </file>
@@ -1695,40 +1716,40 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1810,10 +1831,10 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="C3" s="7">
         <v>3245678</v>
@@ -1824,22 +1845,22 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5">
         <v>22355504</v>
@@ -1847,59 +1868,59 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>10000018</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7">
         <v>412512356</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C8" t="s">
+        <v>276</v>
+      </c>
+      <c r="D8" t="s">
         <v>277</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="F8" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="D8" t="s">
-        <v>279</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>280</v>
-      </c>
       <c r="G8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="31"/>
@@ -1909,22 +1930,22 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B9" s="44">
         <v>46534534</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -1935,10 +1956,10 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C10" s="44">
         <v>46534534</v>
@@ -1949,10 +1970,10 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C11" s="44">
         <v>23444455</v>
@@ -1979,7 +2000,7 @@
   <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2002,40 +2023,40 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>276</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -2052,70 +2073,87 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>298</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>299</v>
+        <v>296</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>345</v>
       </c>
       <c r="C2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" t="s">
         <v>277</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="E2" t="s">
-        <v>279</v>
-      </c>
-      <c r="F2" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>280</v>
-      </c>
       <c r="H2" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
       <c r="I2" t="s">
-        <v>284</v>
+        <v>338</v>
       </c>
       <c r="J2" t="s">
-        <v>283</v>
-      </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
+        <v>339</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>341</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>341</v>
+      </c>
+      <c r="N2" s="31" t="s">
+        <v>322</v>
+      </c>
+      <c r="O2" s="43" t="s">
+        <v>323</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D3" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E3" t="s">
+        <v>277</v>
+      </c>
+      <c r="F3" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="G3" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="H3" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J3" t="s">
         <v>281</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>280</v>
-      </c>
-      <c r="H3" t="s">
-        <v>158</v>
-      </c>
-      <c r="I3" t="s">
-        <v>284</v>
-      </c>
-      <c r="J3" t="s">
-        <v>283</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="32"/>
@@ -2124,147 +2162,147 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D4">
         <v>52486595</v>
       </c>
       <c r="E4" t="s">
+        <v>275</v>
+      </c>
+      <c r="F4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G4" t="s">
         <v>277</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="I4" s="30" t="s">
         <v>278</v>
-      </c>
-      <c r="G4" t="s">
-        <v>279</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="C5" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5" t="s">
         <v>290</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>296</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F5" s="31" t="s">
         <v>291</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" s="30" t="s">
         <v>292</v>
       </c>
-      <c r="E5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F5" s="31" t="s">
+      <c r="H5" t="s">
+        <v>156</v>
+      </c>
+      <c r="I5" t="s">
+        <v>282</v>
+      </c>
+      <c r="J5" t="s">
+        <v>281</v>
+      </c>
+      <c r="K5" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="G5" s="30" t="s">
-        <v>294</v>
-      </c>
-      <c r="H5" t="s">
-        <v>158</v>
-      </c>
-      <c r="I5" t="s">
-        <v>284</v>
-      </c>
-      <c r="J5" t="s">
-        <v>283</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>295</v>
-      </c>
       <c r="L5" s="32" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>297</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="C6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E6" t="s">
+        <v>277</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>300</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>311</v>
-      </c>
-      <c r="C6" t="s">
-        <v>301</v>
-      </c>
-      <c r="D6" t="s">
-        <v>302</v>
-      </c>
-      <c r="E6" t="s">
-        <v>279</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>310</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>303</v>
-      </c>
       <c r="H6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I6" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="J6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="C7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D7" t="s">
+        <v>333</v>
+      </c>
+      <c r="E7" t="s">
+        <v>277</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="H7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I7" t="s">
+        <v>338</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>322</v>
+      </c>
+      <c r="L7" s="43" t="s">
+        <v>323</v>
+      </c>
+      <c r="M7" s="31" t="s">
         <v>324</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>338</v>
-      </c>
-      <c r="C7" t="s">
-        <v>277</v>
-      </c>
-      <c r="D7" t="s">
-        <v>336</v>
-      </c>
-      <c r="E7" t="s">
-        <v>279</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>280</v>
-      </c>
-      <c r="H7" t="s">
-        <v>158</v>
-      </c>
-      <c r="I7" t="s">
-        <v>284</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="K7" s="31" t="s">
+      <c r="N7" s="31" t="s">
         <v>325</v>
-      </c>
-      <c r="L7" s="43" t="s">
-        <v>326</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>327</v>
-      </c>
-      <c r="N7" s="31" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -2298,104 +2336,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D3" s="14">
         <v>10</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4" s="14">
         <v>10</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
       <c r="C5" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="14">
         <v>10</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="14">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2409,7 +2447,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2462,7 +2500,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>8</v>
+        <v>346</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2481,8 +2519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2500,13 +2538,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -2533,14 +2571,16 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7">
-        <v>543416869777</v>
+        <v>346</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2578,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="4"/>
@@ -2606,13 +2646,13 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2655,28 +2695,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>54</v>
-      </c>
       <c r="H1" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>100</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>102</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -2697,1325 +2737,1325 @@
     </row>
     <row r="2" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D2" s="17">
         <v>3413104291</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F2" s="18">
         <v>722341170199331</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D3" s="17">
         <v>3413104292</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F3" s="18">
         <v>722341170199332</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D4" s="17">
         <v>3413104293</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="18">
         <v>722341170199333</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" s="17">
         <v>3413104294</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F5" s="18">
         <v>722341170199334</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D6" s="17">
         <v>3413104295</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F6" s="18">
         <v>722341170199335</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" s="17">
         <v>3413104296</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F7" s="18">
         <v>722341170199336</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D8" s="17">
         <v>3413104297</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F8" s="18">
         <v>722341170199337</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" s="17">
         <v>3413104298</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F9" s="18">
         <v>722341170199338</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D10" s="17">
         <v>3413104299</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F10" s="18">
         <v>722341170199339</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D11" s="17">
         <v>3413104300</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F11" s="18">
         <v>722341170199340</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D12" s="17">
         <v>3413104301</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F12" s="18">
         <v>722341170199341</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D13" s="17">
         <v>3413104302</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F13" s="18">
         <v>722341170199342</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D14" s="17">
         <v>3413104303</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F14" s="18">
         <v>722341170199343</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D15" s="17">
         <v>3413104304</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F15" s="18">
         <v>722341170199344</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D16" s="17">
         <v>3413104305</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F16" s="18">
         <v>722341170199345</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D17" s="17">
         <v>3413104306</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F17" s="18">
         <v>722341170199346</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D18" s="17">
         <v>3413104307</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F18" s="18">
         <v>722341170199347</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D19" s="17">
         <v>3413104308</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F19" s="18">
         <v>722341170199348</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D20" s="17">
         <v>3413104309</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F20" s="18">
         <v>722341170199349</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D21" s="17">
         <v>3413104310</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F21" s="18">
         <v>722341170199350</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D22" s="14">
         <v>3413104311</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F22" s="18">
         <v>722341170199351</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I22" s="18">
         <v>722341170199353</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D23" s="14">
         <v>3413104312</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F23" s="18">
         <v>722341170199352</v>
       </c>
       <c r="G23" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>106</v>
-      </c>
-      <c r="H23" s="19" t="s">
-        <v>108</v>
       </c>
       <c r="I23" s="18">
         <v>722341170199354</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D24" s="14">
         <v>3413104313</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F24" s="18">
         <v>722341170199355</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D25" s="14">
         <v>3413104314</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F25" s="18">
         <v>722341170199356</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C26">
         <v>10000018</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D28" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="G28" s="20" t="s">
         <v>123</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D29" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F29" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>127</v>
-      </c>
-      <c r="F29" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D30" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="G30" s="20" t="s">
         <v>131</v>
-      </c>
-      <c r="F30" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D31" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="G31" s="20" t="s">
         <v>135</v>
-      </c>
-      <c r="F31" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D32" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="G32" s="20" t="s">
         <v>139</v>
-      </c>
-      <c r="F32" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D33" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="G33" s="20" t="s">
         <v>143</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D34" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F34" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="G34" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D35" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>151</v>
-      </c>
-      <c r="F35" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D36" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>155</v>
-      </c>
-      <c r="F36" s="20" t="s">
-        <v>156</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C37" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="F37" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>160</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D38" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38" s="20" t="s">
         <v>163</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>164</v>
-      </c>
-      <c r="F38" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D39" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="F39" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>168</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D40" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="G40" s="20" t="s">
         <v>172</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D41" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="F41" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="G41" s="20" t="s">
         <v>176</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D42" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="F42" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="G42" s="20" t="s">
         <v>180</v>
-      </c>
-      <c r="F42" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D43" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="F43" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="G43" s="20" t="s">
         <v>184</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D44" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="F44" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="G44" s="20" t="s">
         <v>188</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D45" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="F45" s="20" t="s">
         <v>191</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="G45" s="20" t="s">
         <v>192</v>
-      </c>
-      <c r="F45" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D46" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="F46" s="20" t="s">
         <v>195</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="G46" s="20" t="s">
         <v>196</v>
-      </c>
-      <c r="F46" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D47" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="E47" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="F47" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="G47" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="H47" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="I47" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="J47" s="21" t="s">
         <v>203</v>
-      </c>
-      <c r="I47" s="21" t="s">
-        <v>204</v>
-      </c>
-      <c r="J47" s="21" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D48" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="E48" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="F48" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="G48" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="H48" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="I48" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="J48" s="21" t="s">
         <v>210</v>
-      </c>
-      <c r="I48" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="J48" s="21" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D49" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="E49" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="F49" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="G49" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="H49" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="I49" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="H49" s="21" t="s">
+      <c r="J49" s="21" t="s">
         <v>217</v>
-      </c>
-      <c r="I49" s="21" t="s">
-        <v>218</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D50" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="E50" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="F50" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="G50" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="H50" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="I50" s="21" t="s">
         <v>223</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="J50" s="21" t="s">
         <v>224</v>
-      </c>
-      <c r="I50" s="21" t="s">
-        <v>225</v>
-      </c>
-      <c r="J50" s="21" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D51" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="E51" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="F51" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="G51" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="H51" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="I51" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="J51" s="21" t="s">
         <v>231</v>
-      </c>
-      <c r="I51" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="J51" s="21" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D52" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="E52" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="F52" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="G52" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="H52" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="I52" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="H52" s="21" t="s">
+      <c r="J52" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="I52" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="J52" s="21" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D53" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="E53" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="F53" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="G53" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="H53" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="I53" s="21" t="s">
         <v>244</v>
       </c>
-      <c r="H53" s="21" t="s">
+      <c r="J53" s="21" t="s">
         <v>245</v>
-      </c>
-      <c r="I53" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="J53" s="21" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D54" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="E54" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="F54" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="G54" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="H54" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="I54" s="21" t="s">
         <v>251</v>
       </c>
-      <c r="H54" s="21" t="s">
+      <c r="J54" s="21" t="s">
         <v>252</v>
-      </c>
-      <c r="I54" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="J54" s="21" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D55" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="F55" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="G55" s="22" t="s">
         <v>256</v>
-      </c>
-      <c r="F55" s="22" t="s">
-        <v>257</v>
-      </c>
-      <c r="G55" s="22" t="s">
-        <v>258</v>
       </c>
       <c r="H55">
         <v>2514856214</v>
@@ -4023,25 +4063,25 @@
     </row>
     <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D56" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>258</v>
+      </c>
+      <c r="F56" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="G56" s="22" t="s">
         <v>260</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="G56" s="22" t="s">
-        <v>262</v>
       </c>
       <c r="H56">
         <v>2548965321</v>
@@ -4049,13 +4089,13 @@
     </row>
     <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D57" s="22">
         <v>2213104354</v>
@@ -4067,21 +4107,21 @@
         <v>72234</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D58" s="22">
         <v>2213104355</v>
@@ -4093,16 +4133,16 @@
         <v>72235</v>
       </c>
       <c r="G58" s="25" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="H58" s="27" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I58" s="29">
         <v>3</v>
       </c>
       <c r="J58" s="28" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K58" s="26">
         <v>523654</v>
@@ -4118,8 +4158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4141,13 +4181,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -4173,16 +4213,16 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B2" s="38">
         <v>46534534</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E2" s="39">
         <v>1158423198</v>
@@ -4193,7 +4233,7 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B3" s="36">
         <v>23444455</v>
@@ -4206,16 +4246,16 @@
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B4" s="38">
         <v>46534534</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E4" s="39">
         <v>1158423198</v>
@@ -4223,7 +4263,7 @@
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B5" s="41">
         <v>23444455</v>
@@ -4232,19 +4272,19 @@
         <v>123</v>
       </c>
       <c r="D5" s="41" t="s">
+        <v>310</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>311</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>312</v>
+      </c>
+      <c r="G5" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="H5" s="31" t="s">
         <v>314</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>315</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>316</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>317</v>
       </c>
       <c r="I5" s="32">
         <v>4</v>
@@ -4256,73 +4296,73 @@
         <v>1234</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="M5" s="31">
         <v>19784521</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B6" s="37">
         <v>95000022</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B7" s="37">
         <v>95000022</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B8" s="37">
         <v>95000022</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="F8" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B9" s="50">
         <v>12543765</v>
@@ -4347,7 +4387,7 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B10" s="37">
         <v>18766558</v>
@@ -4355,7 +4395,7 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B11" s="37">
         <v>18766558</v>

</xml_diff>

<commit_message>
2018-08-21 - Severl changes
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florangel\git\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Xappia\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Cuenta Normal</t>
   </si>
   <si>
-    <t>Florencia Marketing</t>
-  </si>
-  <si>
     <t>Cuenta c/ Mora</t>
   </si>
   <si>
@@ -1071,6 +1068,9 @@
   </si>
   <si>
     <t>3413105385</t>
+  </si>
+  <si>
+    <t>FaFlorencia Marketing</t>
   </si>
 </sst>
 </file>
@@ -1664,9 +1664,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1719,37 +1719,37 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>347</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1831,10 +1831,10 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="7">
         <v>3245678</v>
@@ -1845,22 +1845,22 @@
     </row>
     <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>18</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>29</v>
       </c>
       <c r="C5">
         <v>22355504</v>
@@ -1868,59 +1868,59 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6">
         <v>10000018</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7">
         <v>412512356</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B8" t="s">
+        <v>274</v>
+      </c>
+      <c r="C8" t="s">
+        <v>275</v>
+      </c>
+      <c r="D8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="G8" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>316</v>
-      </c>
-      <c r="B8" t="s">
-        <v>275</v>
-      </c>
-      <c r="C8" t="s">
-        <v>276</v>
-      </c>
-      <c r="D8" t="s">
-        <v>277</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>279</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="G8" t="s">
-        <v>156</v>
-      </c>
-      <c r="H8" t="s">
-        <v>282</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>317</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="31"/>
@@ -1930,22 +1930,22 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B9" s="44">
         <v>46534534</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -1956,10 +1956,10 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C10" s="44">
         <v>46534534</v>
@@ -1970,10 +1970,10 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C11" s="44">
         <v>23444455</v>
@@ -2023,40 +2023,40 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>274</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -2073,87 +2073,87 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E2" t="s">
         <v>276</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="F2" s="31" t="s">
-        <v>279</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>278</v>
-      </c>
       <c r="H2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
+        <v>337</v>
+      </c>
+      <c r="J2" t="s">
         <v>338</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="32" t="s">
         <v>339</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="L2" s="32" t="s">
         <v>340</v>
       </c>
-      <c r="L2" s="32" t="s">
-        <v>341</v>
-      </c>
       <c r="M2" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N2" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="O2" s="43" t="s">
         <v>322</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="P2" s="31" t="s">
         <v>323</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="Q2" s="31" t="s">
         <v>324</v>
-      </c>
-      <c r="Q2" s="31" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D3" t="s">
         <v>286</v>
       </c>
-      <c r="D3" t="s">
-        <v>287</v>
-      </c>
       <c r="E3" t="s">
+        <v>276</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="G3" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>279</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>278</v>
-      </c>
       <c r="H3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="32"/>
@@ -2162,147 +2162,147 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D4">
         <v>52486595</v>
       </c>
       <c r="E4" t="s">
+        <v>274</v>
+      </c>
+      <c r="F4" t="s">
         <v>275</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>276</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="I4" s="30" t="s">
         <v>277</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>279</v>
-      </c>
-      <c r="I4" s="30" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5" t="s">
         <v>288</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>294</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>289</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>276</v>
+      </c>
+      <c r="F5" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="E5" t="s">
-        <v>277</v>
-      </c>
-      <c r="F5" s="31" t="s">
+      <c r="G5" s="30" t="s">
         <v>291</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="H5" t="s">
+        <v>155</v>
+      </c>
+      <c r="I5" t="s">
+        <v>281</v>
+      </c>
+      <c r="J5" t="s">
+        <v>280</v>
+      </c>
+      <c r="K5" s="32" t="s">
         <v>292</v>
       </c>
-      <c r="H5" t="s">
-        <v>156</v>
-      </c>
-      <c r="I5" t="s">
-        <v>282</v>
-      </c>
-      <c r="J5" t="s">
-        <v>281</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>293</v>
-      </c>
       <c r="L5" s="32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>296</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" t="s">
         <v>297</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>298</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>276</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>299</v>
       </c>
-      <c r="E6" t="s">
-        <v>277</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>300</v>
-      </c>
       <c r="H6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D7" t="s">
+        <v>332</v>
+      </c>
+      <c r="E7" t="s">
+        <v>276</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>278</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="H7" t="s">
+        <v>155</v>
+      </c>
+      <c r="I7" t="s">
+        <v>337</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="K7" s="31" t="s">
         <v>321</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="C7" t="s">
-        <v>275</v>
-      </c>
-      <c r="D7" t="s">
-        <v>333</v>
-      </c>
-      <c r="E7" t="s">
-        <v>277</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>279</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>278</v>
-      </c>
-      <c r="H7" t="s">
-        <v>156</v>
-      </c>
-      <c r="I7" t="s">
-        <v>338</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="K7" s="31" t="s">
+      <c r="L7" s="43" t="s">
         <v>322</v>
       </c>
-      <c r="L7" s="43" t="s">
+      <c r="M7" s="31" t="s">
         <v>323</v>
       </c>
-      <c r="M7" s="31" t="s">
+      <c r="N7" s="31" t="s">
         <v>324</v>
-      </c>
-      <c r="N7" s="31" t="s">
-        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -2336,104 +2336,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" t="s">
-        <v>40</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="14">
         <v>10</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="14">
         <v>10</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="14">
         <v>10</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="14">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2500,7 +2500,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2519,7 +2519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -2538,13 +2538,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -2571,16 +2571,16 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>346</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2618,7 +2618,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="4"/>
@@ -2646,13 +2646,13 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2695,28 +2695,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="G1" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>52</v>
-      </c>
       <c r="H1" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="J1" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>100</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -2737,1325 +2737,1325 @@
     </row>
     <row r="2" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="17">
         <v>3413104291</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F2" s="18">
         <v>722341170199331</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="17">
         <v>3413104292</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="18">
         <v>722341170199332</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="17">
         <v>3413104293</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="18">
         <v>722341170199333</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="17">
         <v>3413104294</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" s="18">
         <v>722341170199334</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="17">
         <v>3413104295</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="18">
         <v>722341170199335</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D7" s="17">
         <v>3413104296</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" s="18">
         <v>722341170199336</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" s="17">
         <v>3413104297</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F8" s="18">
         <v>722341170199337</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D9" s="17">
         <v>3413104298</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" s="18">
         <v>722341170199338</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="17">
         <v>3413104299</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F10" s="18">
         <v>722341170199339</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="17">
         <v>3413104300</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F11" s="18">
         <v>722341170199340</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="17">
         <v>3413104301</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F12" s="18">
         <v>722341170199341</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D13" s="17">
         <v>3413104302</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="18">
         <v>722341170199342</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="17">
         <v>3413104303</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F14" s="18">
         <v>722341170199343</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="17">
         <v>3413104304</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F15" s="18">
         <v>722341170199344</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="17">
         <v>3413104305</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F16" s="18">
         <v>722341170199345</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D17" s="17">
         <v>3413104306</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F17" s="18">
         <v>722341170199346</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D18" s="17">
         <v>3413104307</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F18" s="18">
         <v>722341170199347</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D19" s="17">
         <v>3413104308</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="18">
         <v>722341170199348</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="17">
         <v>3413104309</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F20" s="18">
         <v>722341170199349</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D21" s="17">
         <v>3413104310</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F21" s="18">
         <v>722341170199350</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D22" s="14">
         <v>3413104311</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F22" s="18">
         <v>722341170199351</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I22" s="18">
         <v>722341170199353</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D23" s="14">
         <v>3413104312</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F23" s="18">
         <v>722341170199352</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I23" s="18">
         <v>722341170199354</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D24" s="14">
         <v>3413104313</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F24" s="18">
         <v>722341170199355</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D25" s="14">
         <v>3413104314</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F25" s="18">
         <v>722341170199356</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <v>10000018</v>
       </c>
       <c r="D26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B27" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="D27" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D28" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="E28" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="F28" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="G28" s="20" t="s">
         <v>122</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B29" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D29" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="F29" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>126</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D30" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="F30" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="G30" s="20" t="s">
         <v>130</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B31" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D31" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="F31" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="G31" s="20" t="s">
         <v>134</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B32" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D32" s="20" t="s">
+        <v>135</v>
+      </c>
+      <c r="E32" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="F32" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="G32" s="20" t="s">
         <v>138</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D33" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="F33" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="G33" s="20" t="s">
         <v>142</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D34" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E34" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="F34" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="G34" s="20" t="s">
         <v>146</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D35" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="F35" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>150</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B36" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>115</v>
-      </c>
       <c r="D36" s="20" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="F36" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C37" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="E37" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="F37" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>159</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D38" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="F38" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>163</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D39" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="E39" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="F39" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>167</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D40" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="E40" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="F40" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="F40" s="20" t="s">
+      <c r="G40" s="20" t="s">
         <v>171</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C41" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D41" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E41" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="F41" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="F41" s="20" t="s">
+      <c r="G41" s="20" t="s">
         <v>175</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C42" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D42" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="F42" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="F42" s="20" t="s">
+      <c r="G42" s="20" t="s">
         <v>179</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C43" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D43" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E43" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="F43" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="G43" s="20" t="s">
         <v>183</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D44" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="E44" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="F44" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="G44" s="20" t="s">
         <v>187</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C45" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D45" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="E45" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="F45" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="G45" s="20" t="s">
         <v>191</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D46" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="E46" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="F46" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="G46" s="20" t="s">
         <v>195</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B47" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C47" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="D47" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E47" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="F47" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="G47" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="H47" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="I47" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="I47" s="21" t="s">
+      <c r="J47" s="21" t="s">
         <v>202</v>
-      </c>
-      <c r="J47" s="21" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D48" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="E48" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="F48" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="G48" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="H48" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="I48" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="I48" s="21" t="s">
+      <c r="J48" s="21" t="s">
         <v>209</v>
-      </c>
-      <c r="J48" s="21" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B49" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C49" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="D49" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E49" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="F49" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="G49" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="H49" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="H49" s="21" t="s">
+      <c r="I49" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="I49" s="21" t="s">
+      <c r="J49" s="21" t="s">
         <v>216</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B50" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C50" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="D50" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="E50" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="F50" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="G50" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="H50" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="I50" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="I50" s="21" t="s">
+      <c r="J50" s="21" t="s">
         <v>223</v>
-      </c>
-      <c r="J50" s="21" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B51" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="D51" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="E51" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="F51" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="G51" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="H51" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="I51" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="I51" s="21" t="s">
+      <c r="J51" s="21" t="s">
         <v>230</v>
-      </c>
-      <c r="J51" s="21" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D52" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="E52" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="F52" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="G52" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="H52" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="H52" s="21" t="s">
+      <c r="I52" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="I52" s="21" t="s">
+      <c r="J52" s="21" t="s">
         <v>237</v>
-      </c>
-      <c r="J52" s="21" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D53" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="E53" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="F53" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="G53" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="H53" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="H53" s="21" t="s">
+      <c r="I53" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="I53" s="21" t="s">
+      <c r="J53" s="21" t="s">
         <v>244</v>
-      </c>
-      <c r="J53" s="21" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D54" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="E54" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="F54" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="G54" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="H54" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="H54" s="21" t="s">
+      <c r="I54" s="21" t="s">
         <v>250</v>
       </c>
-      <c r="I54" s="21" t="s">
+      <c r="J54" s="21" t="s">
         <v>251</v>
-      </c>
-      <c r="J54" s="21" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B55" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="C55" s="22" t="s">
-        <v>115</v>
-      </c>
       <c r="D55" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="E55" s="22" t="s">
         <v>253</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="F55" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="F55" s="22" t="s">
+      <c r="G55" s="22" t="s">
         <v>255</v>
-      </c>
-      <c r="G55" s="22" t="s">
-        <v>256</v>
       </c>
       <c r="H55">
         <v>2514856214</v>
@@ -4063,25 +4063,25 @@
     </row>
     <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D56" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="E56" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="F56" s="22" t="s">
         <v>258</v>
       </c>
-      <c r="F56" s="22" t="s">
+      <c r="G56" s="22" t="s">
         <v>259</v>
-      </c>
-      <c r="G56" s="22" t="s">
-        <v>260</v>
       </c>
       <c r="H56">
         <v>2548965321</v>
@@ -4089,13 +4089,13 @@
     </row>
     <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D57" s="22">
         <v>2213104354</v>
@@ -4107,21 +4107,21 @@
         <v>72234</v>
       </c>
       <c r="G57" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="H57" s="24" t="s">
         <v>265</v>
-      </c>
-      <c r="H57" s="24" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D58" s="22">
         <v>2213104355</v>
@@ -4133,16 +4133,16 @@
         <v>72235</v>
       </c>
       <c r="G58" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H58" s="27" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I58" s="29">
         <v>3</v>
       </c>
       <c r="J58" s="28" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K58" s="26">
         <v>523654</v>
@@ -4181,13 +4181,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -4213,16 +4213,16 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B2" s="38">
         <v>46534534</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E2" s="39">
         <v>1158423198</v>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B3" s="36">
         <v>23444455</v>
@@ -4246,16 +4246,16 @@
     </row>
     <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B4" s="38">
         <v>46534534</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E4" s="39">
         <v>1158423198</v>
@@ -4263,7 +4263,7 @@
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B5" s="41">
         <v>23444455</v>
@@ -4272,19 +4272,19 @@
         <v>123</v>
       </c>
       <c r="D5" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="F5" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="G5" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="H5" s="31" t="s">
         <v>313</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>314</v>
       </c>
       <c r="I5" s="32">
         <v>4</v>
@@ -4296,73 +4296,73 @@
         <v>1234</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="M5" s="31">
         <v>19784521</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="37">
         <v>95000022</v>
       </c>
       <c r="C6" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="D6" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="E6" s="48" t="s">
         <v>327</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="45" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7" s="37">
         <v>95000022</v>
       </c>
       <c r="C7" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="D7" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="E7" s="48" t="s">
         <v>327</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B8" s="37">
         <v>95000022</v>
       </c>
       <c r="C8" s="46" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8" s="47" t="s">
         <v>326</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="E8" s="49" t="s">
         <v>327</v>
       </c>
-      <c r="E8" s="49" t="s">
-        <v>328</v>
-      </c>
       <c r="F8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B9" s="50">
         <v>12543765</v>
@@ -4387,7 +4387,7 @@
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B10" s="37">
         <v>18766558</v>
@@ -4395,7 +4395,7 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B11" s="37">
         <v>18766558</v>

</xml_diff>

<commit_message>
PerflogEquip Altas Con equip
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Documents\Teco\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15768" windowHeight="13152" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="347">
   <si>
     <t>Descripción</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Cuenta Activa</t>
   </si>
   <si>
-    <t>Lino Acosta</t>
-  </si>
-  <si>
-    <t>34073327</t>
-  </si>
-  <si>
     <t>Cuenta Activa c/Serv activo</t>
   </si>
   <si>
@@ -950,9 +944,6 @@
     <t>11/04/1989</t>
   </si>
   <si>
-    <t>59885779</t>
-  </si>
-  <si>
     <t>Recargas</t>
   </si>
   <si>
@@ -1071,6 +1062,12 @@
   </si>
   <si>
     <t>FaFlorencia Marketing</t>
+  </si>
+  <si>
+    <t>Alta Linea Equipo Existe</t>
+  </si>
+  <si>
+    <t>59885810</t>
   </si>
 </sst>
 </file>
@@ -1669,16 +1666,16 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1714,42 +1711,42 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1767,19 +1764,19 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1815,26 +1812,26 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>342</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1160444719</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>340</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="7">
         <v>3245678</v>
@@ -1843,84 +1840,84 @@
         <v>1157572274</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>22355504</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>10000018</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>412512356</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B8" t="s">
+        <v>272</v>
+      </c>
+      <c r="C8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D8" t="s">
         <v>274</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="F8" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="D8" t="s">
-        <v>276</v>
-      </c>
-      <c r="E8" s="31" t="s">
-        <v>278</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>277</v>
-      </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="31"/>
@@ -1928,24 +1925,24 @@
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B9" s="44">
         <v>46534534</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -1954,12 +1951,12 @@
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="45" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C10" s="44">
         <v>46534534</v>
@@ -1968,12 +1965,12 @@
         <v>1158423198</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="45" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C11" s="44">
         <v>23444455</v>
@@ -1997,25 +1994,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+    <col min="4" max="5" width="19.44140625" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.33203125" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2023,40 +2020,40 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>273</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -2071,238 +2068,270 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F2" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>112</v>
+      </c>
+      <c r="I2" t="s">
+        <v>334</v>
+      </c>
+      <c r="J2" t="s">
+        <v>335</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>336</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="N2" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="O2" s="43" t="s">
+        <v>319</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" t="s">
+        <v>274</v>
+      </c>
+      <c r="F3" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="G3" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="H3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I3" t="s">
+        <v>279</v>
+      </c>
+      <c r="J3" t="s">
         <v>278</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="H2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I2" t="s">
-        <v>337</v>
-      </c>
-      <c r="J2" t="s">
-        <v>338</v>
-      </c>
-      <c r="K2" s="32" t="s">
-        <v>339</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>340</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>340</v>
-      </c>
-      <c r="N2" s="31" t="s">
-        <v>321</v>
-      </c>
-      <c r="O2" s="43" t="s">
-        <v>322</v>
-      </c>
-      <c r="P2" s="31" t="s">
-        <v>323</v>
-      </c>
-      <c r="Q2" s="31" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>294</v>
-      </c>
-      <c r="C3" t="s">
-        <v>285</v>
-      </c>
-      <c r="D3" t="s">
-        <v>286</v>
-      </c>
-      <c r="E3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>278</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="H3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I3" t="s">
-        <v>281</v>
-      </c>
-      <c r="J3" t="s">
-        <v>280</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="32"/>
       <c r="M3" s="32"/>
       <c r="N3" s="32"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D4">
         <v>52486595</v>
       </c>
       <c r="E4" t="s">
+        <v>272</v>
+      </c>
+      <c r="F4" t="s">
+        <v>273</v>
+      </c>
+      <c r="G4" t="s">
         <v>274</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="I4" s="30" t="s">
         <v>275</v>
       </c>
-      <c r="G4" t="s">
-        <v>276</v>
-      </c>
-      <c r="H4" s="31" t="s">
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" t="s">
+        <v>286</v>
+      </c>
+      <c r="D5" t="s">
+        <v>287</v>
+      </c>
+      <c r="E5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="H5" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" t="s">
+        <v>279</v>
+      </c>
+      <c r="J5" t="s">
         <v>278</v>
       </c>
-      <c r="I4" s="30" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>287</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="C5" t="s">
-        <v>288</v>
-      </c>
-      <c r="D5" t="s">
-        <v>289</v>
-      </c>
-      <c r="E5" t="s">
-        <v>276</v>
-      </c>
-      <c r="F5" s="31" t="s">
+      <c r="K5" s="32" t="s">
         <v>290</v>
       </c>
-      <c r="G5" s="30" t="s">
-        <v>291</v>
-      </c>
-      <c r="H5" t="s">
-        <v>155</v>
-      </c>
-      <c r="I5" t="s">
-        <v>281</v>
-      </c>
-      <c r="J5" t="s">
-        <v>280</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>292</v>
-      </c>
       <c r="L5" s="32" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="C6" t="s">
+        <v>295</v>
+      </c>
+      <c r="D6" t="s">
         <v>296</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
+        <v>274</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>304</v>
+      </c>
+      <c r="G6" s="33" t="s">
         <v>297</v>
       </c>
-      <c r="D6" t="s">
-        <v>298</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="H6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" t="s">
+        <v>334</v>
+      </c>
+      <c r="J6" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="C7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D7" t="s">
+        <v>329</v>
+      </c>
+      <c r="E7" t="s">
+        <v>274</v>
+      </c>
+      <c r="F7" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="F6" s="32" t="s">
-        <v>306</v>
-      </c>
-      <c r="G6" s="33" t="s">
-        <v>299</v>
-      </c>
-      <c r="H6" t="s">
-        <v>155</v>
-      </c>
-      <c r="I6" t="s">
-        <v>281</v>
-      </c>
-      <c r="J6" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="G7" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="H7" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" t="s">
+        <v>334</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>318</v>
+      </c>
+      <c r="L7" s="43" t="s">
+        <v>319</v>
+      </c>
+      <c r="M7" s="31" t="s">
         <v>320</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="N7" s="31" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>345</v>
+      </c>
+      <c r="B8">
+        <v>59885136</v>
+      </c>
+      <c r="C8" t="s">
+        <v>339</v>
+      </c>
+      <c r="D8" t="s">
+        <v>273</v>
+      </c>
+      <c r="E8" t="s">
+        <v>274</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="H8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I8" t="s">
         <v>334</v>
       </c>
-      <c r="C7" t="s">
-        <v>274</v>
-      </c>
-      <c r="D7" t="s">
-        <v>332</v>
-      </c>
-      <c r="E7" t="s">
-        <v>276</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>278</v>
-      </c>
-      <c r="G7" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="H7" t="s">
-        <v>155</v>
-      </c>
-      <c r="I7" t="s">
-        <v>337</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="K7" s="31" t="s">
-        <v>321</v>
-      </c>
-      <c r="L7" s="43" t="s">
-        <v>322</v>
-      </c>
-      <c r="M7" s="31" t="s">
-        <v>323</v>
-      </c>
-      <c r="N7" s="31" t="s">
-        <v>324</v>
+      <c r="J8" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -2327,113 +2356,113 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="5" max="5" width="36.140625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="36.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
       </c>
       <c r="D2">
         <v>10</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D3" s="14">
         <v>10</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="14">
         <v>10</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
       <c r="C5" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D5" s="14">
         <v>10</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="14">
         <v>10</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2450,16 +2479,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2495,12 +2524,12 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2520,31 +2549,31 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
+    <col min="5" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
@@ -2569,18 +2598,18 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>343</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>346</v>
       </c>
     </row>
   </sheetData>
@@ -2601,16 +2630,16 @@
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
-    <col min="4" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2618,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="4"/>
@@ -2644,15 +2673,15 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -2673,21 +2702,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.140625" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" customWidth="1"/>
-    <col min="6" max="6" width="25.28515625" customWidth="1"/>
-    <col min="7" max="7" width="38.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" customWidth="1"/>
-    <col min="10" max="10" width="40.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="29.109375" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="7" max="7" width="38.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.5546875" customWidth="1"/>
+    <col min="9" max="9" width="23.44140625" customWidth="1"/>
+    <col min="10" max="10" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2695,28 +2724,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>51</v>
-      </c>
       <c r="H1" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>97</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>99</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -2735,1367 +2764,1367 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D2" s="17">
         <v>3413104291</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" s="18">
         <v>722341170199331</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D3" s="17">
         <v>3413104292</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" s="18">
         <v>722341170199332</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D4" s="17">
         <v>3413104293</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" s="18">
         <v>722341170199333</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="17">
         <v>3413104294</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F5" s="18">
         <v>722341170199334</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6" s="17">
         <v>3413104295</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F6" s="18">
         <v>722341170199335</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D7" s="17">
         <v>3413104296</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F7" s="18">
         <v>722341170199336</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="17">
         <v>3413104297</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F8" s="18">
         <v>722341170199337</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D9" s="17">
         <v>3413104298</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F9" s="18">
         <v>722341170199338</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10" s="17">
         <v>3413104299</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F10" s="18">
         <v>722341170199339</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D11" s="17">
         <v>3413104300</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F11" s="18">
         <v>722341170199340</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D12" s="17">
         <v>3413104301</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F12" s="18">
         <v>722341170199341</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D13" s="17">
         <v>3413104302</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F13" s="18">
         <v>722341170199342</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="17">
         <v>3413104303</v>
       </c>
       <c r="E14" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F14" s="18">
         <v>722341170199343</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D15" s="17">
         <v>3413104304</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F15" s="18">
         <v>722341170199344</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D16" s="17">
         <v>3413104305</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" s="18">
         <v>722341170199345</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="17">
         <v>3413104306</v>
       </c>
       <c r="E17" s="19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F17" s="18">
         <v>722341170199346</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D18" s="17">
         <v>3413104307</v>
       </c>
       <c r="E18" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F18" s="18">
         <v>722341170199347</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D19" s="17">
         <v>3413104308</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F19" s="18">
         <v>722341170199348</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20" s="17">
         <v>3413104309</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F20" s="18">
         <v>722341170199349</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D21" s="17">
         <v>3413104310</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F21" s="18">
         <v>722341170199350</v>
       </c>
       <c r="G21" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>73</v>
       </c>
       <c r="D22" s="14">
         <v>3413104311</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F22" s="18">
         <v>722341170199351</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I22" s="18">
         <v>722341170199353</v>
       </c>
       <c r="J22" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>108</v>
-      </c>
       <c r="B23" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D23" s="14">
         <v>3413104312</v>
       </c>
       <c r="E23" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F23" s="18">
         <v>722341170199352</v>
       </c>
       <c r="G23" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="H23" s="19" t="s">
-        <v>105</v>
       </c>
       <c r="I23" s="18">
         <v>722341170199354</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D24" s="14">
         <v>3413104313</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F24" s="18">
         <v>722341170199355</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" s="14">
         <v>3413104314</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F25" s="18">
         <v>722341170199356</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>10000018</v>
       </c>
       <c r="D26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B27" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="F27" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="20" t="s">
+    </row>
+    <row r="28" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="E28" s="20" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C28" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D28" s="20" t="s">
+      <c r="F28" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="G28" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="F28" s="20" t="s">
+    </row>
+    <row r="29" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="E29" s="20" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D29" s="20" t="s">
+      <c r="F29" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="F29" s="20" t="s">
+    </row>
+    <row r="30" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="G29" s="20" t="s">
+      <c r="E30" s="20" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" s="20" t="s">
+      <c r="F30" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="G30" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="F30" s="20" t="s">
+    </row>
+    <row r="31" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="G30" s="20" t="s">
+      <c r="E31" s="20" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" s="20" t="s">
+      <c r="F31" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="20" t="s">
+      <c r="G31" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="F31" s="20" t="s">
+    </row>
+    <row r="32" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="G31" s="20" t="s">
+      <c r="E32" s="20" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D32" s="20" t="s">
+      <c r="F32" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="G32" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="F32" s="20" t="s">
+    </row>
+    <row r="33" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="E33" s="20" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D33" s="20" t="s">
+      <c r="F33" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="G33" s="20" t="s">
         <v>140</v>
       </c>
-      <c r="F33" s="20" t="s">
+    </row>
+    <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D34" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="E34" s="20" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C34" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" s="20" t="s">
+      <c r="F34" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="G34" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="F34" s="20" t="s">
+    </row>
+    <row r="35" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="20" t="s">
         <v>145</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="E35" s="20" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B35" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" s="20" t="s">
+      <c r="F35" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>148</v>
       </c>
-      <c r="F35" s="20" t="s">
+    </row>
+    <row r="36" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="E36" s="20" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="20" t="s">
+      <c r="F36" s="20" t="s">
         <v>151</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>152</v>
       </c>
-      <c r="F36" s="20" t="s">
+    </row>
+    <row r="37" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>153</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="D37" s="20" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C37" s="20" t="s">
+      <c r="E37" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="F37" s="20" t="s">
         <v>156</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="F37" s="20" t="s">
+    </row>
+    <row r="38" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D38" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="E38" s="20" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C38" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D38" s="20" t="s">
+      <c r="F38" s="20" t="s">
         <v>160</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="F38" s="20" t="s">
+    </row>
+    <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D39" s="20" t="s">
         <v>162</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="E39" s="20" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C39" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D39" s="20" t="s">
+      <c r="F39" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>165</v>
       </c>
-      <c r="F39" s="20" t="s">
+    </row>
+    <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D40" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="E40" s="20" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C40" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D40" s="20" t="s">
+      <c r="F40" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="G40" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="F40" s="20" t="s">
+    </row>
+    <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="E41" s="20" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D41" s="20" t="s">
+      <c r="F41" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="G41" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="F41" s="20" t="s">
+    </row>
+    <row r="42" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="E42" s="20" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D42" s="20" t="s">
+      <c r="F42" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="G42" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="F42" s="20" t="s">
+    </row>
+    <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D43" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="E43" s="20" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D43" s="20" t="s">
+      <c r="F43" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="G43" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="F43" s="20" t="s">
+    </row>
+    <row r="44" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D44" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="G43" s="20" t="s">
+      <c r="E44" s="20" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" s="20" t="s">
+      <c r="F44" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="G44" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="F44" s="20" t="s">
+    </row>
+    <row r="45" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="E45" s="20" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C45" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="20" t="s">
+      <c r="F45" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="G45" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="F45" s="20" t="s">
+    </row>
+    <row r="46" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="G45" s="20" t="s">
+      <c r="E46" s="20" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="B46" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C46" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="D46" s="20" t="s">
+      <c r="F46" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="E46" s="20" t="s">
+      <c r="G46" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="F46" s="20" t="s">
+    </row>
+    <row r="47" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="21" t="s">
         <v>194</v>
       </c>
-      <c r="G46" s="20" t="s">
+      <c r="E47" s="21" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D47" s="21" t="s">
+      <c r="F47" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="E47" s="21" t="s">
+      <c r="G47" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="F47" s="21" t="s">
+      <c r="H47" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="G47" s="21" t="s">
+      <c r="I47" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="H47" s="21" t="s">
+      <c r="J47" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="I47" s="21" t="s">
+    </row>
+    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D48" s="21" t="s">
         <v>201</v>
       </c>
-      <c r="J47" s="21" t="s">
+      <c r="E48" s="21" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="B48" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C48" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D48" s="21" t="s">
+      <c r="F48" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="G48" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="F48" s="21" t="s">
+      <c r="H48" s="21" t="s">
         <v>205</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="I48" s="21" t="s">
         <v>206</v>
       </c>
-      <c r="H48" s="21" t="s">
+      <c r="J48" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="I48" s="21" t="s">
+    </row>
+    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" s="21" t="s">
         <v>208</v>
       </c>
-      <c r="J48" s="21" t="s">
+      <c r="E49" s="21" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B49" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D49" s="21" t="s">
+      <c r="F49" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="G49" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="H49" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="I49" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="H49" s="21" t="s">
+      <c r="J49" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="I49" s="21" t="s">
+    </row>
+    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D50" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="J49" s="21" t="s">
+      <c r="E50" s="21" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B50" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D50" s="21" t="s">
+      <c r="F50" s="21" t="s">
         <v>217</v>
       </c>
-      <c r="E50" s="21" t="s">
+      <c r="G50" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="F50" s="21" t="s">
+      <c r="H50" s="21" t="s">
         <v>219</v>
       </c>
-      <c r="G50" s="21" t="s">
+      <c r="I50" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="H50" s="21" t="s">
+      <c r="J50" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="I50" s="21" t="s">
+    </row>
+    <row r="51" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D51" s="21" t="s">
         <v>222</v>
       </c>
-      <c r="J50" s="21" t="s">
+      <c r="E51" s="21" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B51" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C51" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="D51" s="21" t="s">
+      <c r="F51" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="E51" s="21" t="s">
+      <c r="G51" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="F51" s="21" t="s">
+      <c r="H51" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="G51" s="21" t="s">
+      <c r="I51" s="21" t="s">
         <v>227</v>
       </c>
-      <c r="H51" s="21" t="s">
+      <c r="J51" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="I51" s="21" t="s">
+    </row>
+    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A52" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="J51" s="21" t="s">
+      <c r="E52" s="21" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B52" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C52" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D52" s="21" t="s">
+      <c r="F52" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="G52" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="F52" s="21" t="s">
+      <c r="H52" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="G52" s="21" t="s">
+      <c r="I52" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="H52" s="21" t="s">
+      <c r="J52" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="I52" s="21" t="s">
+    </row>
+    <row r="53" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A53" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="21" t="s">
         <v>236</v>
       </c>
-      <c r="J52" s="21" t="s">
+      <c r="E53" s="21" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B53" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C53" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D53" s="21" t="s">
+      <c r="F53" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="E53" s="21" t="s">
+      <c r="G53" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="F53" s="21" t="s">
+      <c r="H53" s="21" t="s">
         <v>240</v>
       </c>
-      <c r="G53" s="21" t="s">
+      <c r="I53" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="H53" s="21" t="s">
+      <c r="J53" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="I53" s="21" t="s">
+    </row>
+    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="J53" s="21" t="s">
+      <c r="E54" s="21" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B54" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="D54" s="21" t="s">
+      <c r="F54" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="G54" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="F54" s="21" t="s">
+      <c r="H54" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="G54" s="21" t="s">
+      <c r="I54" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="H54" s="21" t="s">
+      <c r="J54" s="21" t="s">
         <v>249</v>
       </c>
-      <c r="I54" s="21" t="s">
+    </row>
+    <row r="55" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A55" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D55" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="J54" s="21" t="s">
+      <c r="E55" s="22" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>113</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="D55" s="22" t="s">
+      <c r="F55" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="E55" s="22" t="s">
+      <c r="G55" s="22" t="s">
         <v>253</v>
-      </c>
-      <c r="F55" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="G55" s="22" t="s">
-        <v>255</v>
       </c>
       <c r="H55">
         <v>2514856214</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D56" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="F56" s="22" t="s">
         <v>256</v>
       </c>
-      <c r="E56" s="22" t="s">
+      <c r="G56" s="22" t="s">
         <v>257</v>
-      </c>
-      <c r="F56" s="22" t="s">
-        <v>258</v>
-      </c>
-      <c r="G56" s="22" t="s">
-        <v>259</v>
       </c>
       <c r="H56">
         <v>2548965321</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D57" s="22">
         <v>2213104354</v>
@@ -4107,21 +4136,21 @@
         <v>72234</v>
       </c>
       <c r="G57" s="23" t="s">
+        <v>262</v>
+      </c>
+      <c r="H57" s="24" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="14" t="s">
         <v>264</v>
       </c>
-      <c r="H57" s="24" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
-        <v>266</v>
-      </c>
       <c r="B58" s="23" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D58" s="22">
         <v>2213104355</v>
@@ -4133,16 +4162,16 @@
         <v>72235</v>
       </c>
       <c r="G58" s="25" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="H58" s="27" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I58" s="29">
         <v>3</v>
       </c>
       <c r="J58" s="28" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K58" s="26">
         <v>523654</v>
@@ -4158,22 +4187,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="14" width="11.5546875" customWidth="1"/>
+    <col min="15" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4181,13 +4210,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="E1" s="35" t="s">
         <v>302</v>
-      </c>
-      <c r="E1" s="35" t="s">
-        <v>304</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -4211,29 +4240,29 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B2" s="38">
         <v>46534534</v>
       </c>
       <c r="C2" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>301</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>303</v>
       </c>
       <c r="E2" s="39">
         <v>1158423198</v>
       </c>
       <c r="F2">
-        <v>1161138551</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1161135555</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B3" s="36">
         <v>23444455</v>
@@ -4241,29 +4270,29 @@
       <c r="C3" s="40"/>
       <c r="D3" s="41"/>
       <c r="G3">
-        <v>1161138552</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1161135555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B4" s="38">
         <v>46534534</v>
       </c>
       <c r="C4" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="D4" s="37" t="s">
         <v>301</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>303</v>
       </c>
       <c r="E4" s="39">
         <v>1158423198</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B5" s="41">
         <v>23444455</v>
@@ -4272,19 +4301,19 @@
         <v>123</v>
       </c>
       <c r="D5" s="41" t="s">
+        <v>306</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>307</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="G5" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="H5" s="31" t="s">
         <v>310</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>311</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>312</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>313</v>
       </c>
       <c r="I5" s="32">
         <v>4</v>
@@ -4296,75 +4325,75 @@
         <v>1234</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="M5" s="31">
         <v>19784521</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="O5" s="14"/>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="45" t="s">
+        <v>325</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="D7" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="45" t="s">
+        <v>327</v>
+      </c>
+      <c r="B8" s="37">
+        <v>95000022</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>322</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>323</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>324</v>
+      </c>
+      <c r="F8" t="s">
         <v>328</v>
       </c>
-      <c r="B6" s="37">
-        <v>95000022</v>
-      </c>
-      <c r="C6" s="46" t="s">
-        <v>325</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>326</v>
-      </c>
-      <c r="E6" s="48" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="45" t="s">
-        <v>329</v>
-      </c>
-      <c r="B7" s="37">
-        <v>95000022</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>325</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>326</v>
-      </c>
-      <c r="E7" s="48" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="45" t="s">
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
         <v>330</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>343</v>
-      </c>
-      <c r="C8" s="46" t="s">
-        <v>325</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>326</v>
-      </c>
-      <c r="E8" s="49" t="s">
-        <v>327</v>
-      </c>
-      <c r="F8" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="31" t="s">
-        <v>333</v>
-      </c>
-      <c r="B9" s="37">
+      <c r="B9" s="50">
         <v>12543765</v>
       </c>
       <c r="C9" s="42">
@@ -4385,17 +4414,17 @@
       <c r="N9" s="31"/>
       <c r="O9" s="14"/>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B10" s="37">
         <v>18766558</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B11" s="37">
         <v>18766558</v>

</xml_diff>

<commit_message>
archivo cuentas para uat
si van a correr algo en uat solo se debe cambiar el nombre de los arcivos y listo
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofia Chardin\Git\TelecomProyectoFAN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florangel\git\TelecomProyectoFAN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15768" windowHeight="13152" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="13155" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="379">
   <si>
     <t>Descripción</t>
   </si>
@@ -939,9 +939,6 @@
   </si>
   <si>
     <t>Alta Linea Nuevo Agente Presencial</t>
-  </si>
-  <si>
-    <t>VICENTE LOPEZ</t>
   </si>
   <si>
     <t>Alta Linea Existente OfCom Presencial</t>
@@ -1405,7 +1402,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1479,7 +1476,6 @@
     <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1773,16 +1769,16 @@
       <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1818,17 +1814,17 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1838,7 +1834,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1848,7 +1844,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1871,19 +1867,19 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1919,7 +1915,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1933,7 +1929,7 @@
         <v>1160444719</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1947,7 +1943,7 @@
         <v>1157572274</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -1959,7 +1955,7 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1970,7 +1966,7 @@
         <v>22355504</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1984,7 +1980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1998,7 +1994,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>303</v>
       </c>
@@ -2018,13 +2014,13 @@
         <v>277</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
-        <v>280</v>
+        <v>321</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="31"/>
@@ -2032,9 +2028,9 @@
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B9" s="44">
         <v>46534534</v>
@@ -2043,13 +2039,13 @@
         <v>277</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="E9" t="s">
-        <v>280</v>
+        <v>321</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
@@ -2058,9 +2054,9 @@
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B10" s="44" t="s">
         <v>296</v>
@@ -2072,9 +2068,9 @@
         <v>1158423198</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B11" s="44" t="s">
         <v>300</v>
@@ -2105,28 +2101,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" customWidth="1"/>
-    <col min="4" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="8" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2182,15 +2178,15 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>294</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D2" t="s">
         <v>275</v>
@@ -2208,34 +2204,34 @@
         <v>114</v>
       </c>
       <c r="I2" t="s">
+        <v>321</v>
+      </c>
+      <c r="J2" t="s">
         <v>322</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="32" t="s">
         <v>323</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="L2" s="32" t="s">
         <v>324</v>
       </c>
-      <c r="L2" s="32" t="s">
-        <v>325</v>
-      </c>
       <c r="M2" s="32" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="N2" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="O2" s="43" t="s">
         <v>309</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="P2" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="Q2" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="Q2" s="31" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -2271,7 +2267,7 @@
       <c r="M3" s="32"/>
       <c r="N3" s="32"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>260</v>
       </c>
@@ -2279,7 +2275,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D4">
         <v>52486595</v>
@@ -2300,7 +2296,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>286</v>
       </c>
@@ -2326,10 +2322,10 @@
         <v>114</v>
       </c>
       <c r="I5" t="s">
-        <v>280</v>
+        <v>321</v>
       </c>
       <c r="J5" t="s">
-        <v>279</v>
+        <v>322</v>
       </c>
       <c r="K5" s="32" t="s">
         <v>291</v>
@@ -2340,18 +2336,18 @@
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B6" s="31" t="s">
+        <v>358</v>
+      </c>
+      <c r="C6" t="s">
         <v>359</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>360</v>
-      </c>
-      <c r="D6" t="s">
-        <v>361</v>
       </c>
       <c r="E6" t="s">
         <v>276</v>
@@ -2366,45 +2362,45 @@
         <v>114</v>
       </c>
       <c r="I6" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K6" s="31" t="s">
+        <v>308</v>
+      </c>
+      <c r="L6" s="43" t="s">
         <v>309</v>
       </c>
-      <c r="L6" s="43" t="s">
+      <c r="M6" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="M6" s="31" t="s">
+      <c r="N6" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="N6" s="31" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B7">
         <v>59886004</v>
       </c>
       <c r="C7" t="s">
+        <v>361</v>
+      </c>
+      <c r="D7" t="s">
         <v>362</v>
-      </c>
-      <c r="D7" t="s">
-        <v>363</v>
       </c>
       <c r="E7" t="s">
         <v>276</v>
       </c>
-      <c r="F7" s="53">
-        <v>32016</v>
+      <c r="F7" s="31" t="s">
+        <v>289</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H7" t="s">
         <v>114</v>
@@ -2413,10 +2409,10 @@
         <v>280</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L7">
         <v>1524</v>
@@ -2425,45 +2421,45 @@
         <v>1524</v>
       </c>
       <c r="N7" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="R7" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="O7" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="P7" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q7" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="R7" s="31" t="s">
+      <c r="S7" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="S7" s="31" t="s">
+      <c r="T7" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="T7" s="31" t="s">
+      <c r="U7" s="31" t="s">
         <v>340</v>
-      </c>
-      <c r="U7" s="31" t="s">
-        <v>341</v>
       </c>
       <c r="V7" s="31"/>
       <c r="W7" s="31"/>
       <c r="X7" s="46"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C8" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" t="s">
         <v>351</v>
-      </c>
-      <c r="D8" t="s">
-        <v>352</v>
       </c>
       <c r="E8" t="s">
         <v>276</v>
@@ -2472,19 +2468,19 @@
         <v>278</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H8" t="s">
         <v>114</v>
       </c>
       <c r="I8" t="s">
+        <v>321</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>323</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>324</v>
       </c>
       <c r="L8">
         <v>1524</v>
@@ -2493,16 +2489,16 @@
         <v>1524</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B9" s="32"/>
       <c r="C9" t="s">
+        <v>365</v>
+      </c>
+      <c r="D9" t="s">
         <v>366</v>
-      </c>
-      <c r="D9" t="s">
-        <v>367</v>
       </c>
       <c r="E9" t="s">
         <v>276</v>
@@ -2511,19 +2507,19 @@
         <v>278</v>
       </c>
       <c r="G9" s="33" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H9" t="s">
         <v>114</v>
       </c>
       <c r="I9" t="s">
+        <v>321</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="K9" s="31" t="s">
         <v>323</v>
-      </c>
-      <c r="K9" s="31" t="s">
-        <v>324</v>
       </c>
       <c r="L9">
         <v>1544</v>
@@ -2532,69 +2528,69 @@
         <v>1524</v>
       </c>
       <c r="N9" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="O9" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="P9" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q9" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="R9" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="O9" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="P9" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q9" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="R9" s="31" t="s">
+      <c r="S9" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="S9" s="31" t="s">
+      <c r="T9" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="T9" s="31" t="s">
+      <c r="U9" s="31" t="s">
         <v>340</v>
-      </c>
-      <c r="U9" s="31" t="s">
-        <v>341</v>
       </c>
       <c r="V9" s="31" t="s">
         <v>302</v>
       </c>
       <c r="W9" s="31" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="X9" s="46" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>376</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E10" t="s">
+        <v>378</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="G10" s="33" t="s">
         <v>345</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>377</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="E10" t="s">
-        <v>379</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>346</v>
       </c>
       <c r="H10" t="s">
         <v>114</v>
       </c>
       <c r="I10" t="s">
+        <v>321</v>
+      </c>
+      <c r="J10" t="s">
         <v>322</v>
-      </c>
-      <c r="J10" t="s">
-        <v>323</v>
       </c>
       <c r="K10" s="49"/>
     </row>
@@ -2622,14 +2618,14 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="36.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>37</v>
       </c>
@@ -2646,7 +2642,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>40</v>
       </c>
@@ -2663,7 +2659,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>41</v>
       </c>
@@ -2680,7 +2676,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>43</v>
       </c>
@@ -2697,7 +2693,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -2714,7 +2710,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="14" t="s">
         <v>43</v>
       </c>
@@ -2745,16 +2741,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2790,12 +2786,12 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -2818,17 +2814,17 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="14" width="11.5546875" customWidth="1"/>
-    <col min="15" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2864,18 +2860,18 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>330</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -2896,16 +2892,16 @@
       <selection activeCell="A1000" sqref="A3:XFD1000"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="4" max="13" width="11.5546875" customWidth="1"/>
-    <col min="14" max="26" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2939,7 +2935,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2968,21 +2964,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
-    <col min="7" max="7" width="38.33203125" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" customWidth="1"/>
-    <col min="9" max="9" width="23.44140625" customWidth="1"/>
-    <col min="10" max="10" width="40.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.140625" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.42578125" customWidth="1"/>
+    <col min="10" max="10" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3030,7 +3026,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>76</v>
       </c>
@@ -3053,7 +3049,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>76</v>
       </c>
@@ -3076,7 +3072,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>76</v>
       </c>
@@ -3099,7 +3095,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>76</v>
       </c>
@@ -3122,7 +3118,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>76</v>
       </c>
@@ -3145,7 +3141,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>76</v>
       </c>
@@ -3168,7 +3164,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>76</v>
       </c>
@@ -3191,7 +3187,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>76</v>
       </c>
@@ -3214,7 +3210,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>76</v>
       </c>
@@ -3237,7 +3233,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>76</v>
       </c>
@@ -3260,7 +3256,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>76</v>
       </c>
@@ -3283,7 +3279,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>76</v>
       </c>
@@ -3306,7 +3302,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>76</v>
       </c>
@@ -3329,7 +3325,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>76</v>
       </c>
@@ -3352,7 +3348,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>76</v>
       </c>
@@ -3375,7 +3371,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>76</v>
       </c>
@@ -3398,7 +3394,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>76</v>
       </c>
@@ -3421,7 +3417,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>76</v>
       </c>
@@ -3444,7 +3440,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>76</v>
       </c>
@@ -3467,7 +3463,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>76</v>
       </c>
@@ -3490,7 +3486,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>108</v>
       </c>
@@ -3522,7 +3518,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>108</v>
       </c>
@@ -3554,7 +3550,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>76</v>
       </c>
@@ -3577,7 +3573,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>76</v>
       </c>
@@ -3600,7 +3596,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>260</v>
       </c>
@@ -3614,7 +3610,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>76</v>
       </c>
@@ -3637,7 +3633,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
@@ -3660,7 +3656,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>76</v>
       </c>
@@ -3683,7 +3679,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>76</v>
       </c>
@@ -3706,7 +3702,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>76</v>
       </c>
@@ -3729,7 +3725,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>76</v>
       </c>
@@ -3752,7 +3748,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>76</v>
       </c>
@@ -3775,7 +3771,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>76</v>
       </c>
@@ -3798,7 +3794,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>76</v>
       </c>
@@ -3821,7 +3817,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>76</v>
       </c>
@@ -3844,7 +3840,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>76</v>
       </c>
@@ -3867,7 +3863,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>76</v>
       </c>
@@ -3890,7 +3886,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>76</v>
       </c>
@@ -3913,7 +3909,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
         <v>76</v>
       </c>
@@ -3936,7 +3932,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>76</v>
       </c>
@@ -3959,7 +3955,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>76</v>
       </c>
@@ -3982,7 +3978,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>76</v>
       </c>
@@ -4005,7 +4001,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>76</v>
       </c>
@@ -4028,7 +4024,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>76</v>
       </c>
@@ -4051,7 +4047,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>76</v>
       </c>
@@ -4074,7 +4070,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>108</v>
       </c>
@@ -4106,7 +4102,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>108</v>
       </c>
@@ -4138,7 +4134,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>261</v>
       </c>
@@ -4170,7 +4166,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>261</v>
       </c>
@@ -4202,7 +4198,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
         <v>261</v>
       </c>
@@ -4234,7 +4230,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="14" t="s">
         <v>261</v>
       </c>
@@ -4266,7 +4262,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>261</v>
       </c>
@@ -4298,7 +4294,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="14" t="s">
         <v>261</v>
       </c>
@@ -4330,7 +4326,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>262</v>
       </c>
@@ -4356,7 +4352,7 @@
         <v>2514856214</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>262</v>
       </c>
@@ -4382,7 +4378,7 @@
         <v>2548965321</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="14" t="s">
         <v>75</v>
       </c>
@@ -4408,7 +4404,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>266</v>
       </c>
@@ -4453,26 +4449,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="11.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="11.5703125" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="26" width="9.109375" customWidth="1"/>
+    <col min="16" max="26" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4510,7 +4506,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>286</v>
       </c>
@@ -4530,7 +4526,7 @@
         <v>1161138551</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
         <v>286</v>
       </c>
@@ -4543,7 +4539,7 @@
         <v>1161138552</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>296</v>
       </c>
@@ -4560,39 +4556,39 @@
         <v>1158423198</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
         <v>301</v>
       </c>
       <c r="B5" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" s="52" t="s">
         <v>369</v>
       </c>
-      <c r="C5" s="52" t="s">
-        <v>370</v>
-      </c>
       <c r="D5" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="H5" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="H5" s="31" t="s">
+      <c r="I5" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="J5" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="K5" s="31" t="s">
         <v>340</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>341</v>
       </c>
       <c r="L5" s="31" t="s">
         <v>302</v>
@@ -4607,71 +4603,71 @@
         <v>3463406620</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>369</v>
+      </c>
+      <c r="D6" s="47" t="s">
+        <v>370</v>
+      </c>
+      <c r="E6" s="51" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B7" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C7" s="52" t="s">
         <v>369</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="D7" s="47" t="s">
         <v>370</v>
       </c>
-      <c r="D6" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
+      <c r="E7" s="51" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B8" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C8" s="52" t="s">
         <v>369</v>
       </c>
-      <c r="C7" s="52" t="s">
-        <v>370</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="E7" s="51" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="D8" s="47" t="s">
+        <v>312</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>313</v>
+      </c>
+      <c r="F8" t="s">
         <v>317</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>370</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>313</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>314</v>
-      </c>
-      <c r="F8" t="s">
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="31" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>319</v>
-      </c>
       <c r="B9" s="37" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C9" s="42">
         <v>123</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="54">
         <v>1515151515</v>
       </c>
       <c r="E9" s="31"/>
@@ -4686,112 +4682,112 @@
       <c r="N9" s="31"/>
       <c r="O9" s="14"/>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="45" t="s">
+        <v>319</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="45" t="s">
         <v>320</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
-        <v>321</v>
-      </c>
       <c r="B11" s="37" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B12" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C12" s="52" t="s">
         <v>369</v>
       </c>
-      <c r="C12" s="52" t="s">
-        <v>370</v>
-      </c>
       <c r="D12" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="H12" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="E12" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="H12" s="31" t="s">
+      <c r="I12" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="I12" s="31" t="s">
+      <c r="J12" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="K12" s="31" t="s">
         <v>340</v>
-      </c>
-      <c r="K12" s="31" t="s">
-        <v>341</v>
       </c>
       <c r="L12" s="31" t="s">
         <v>302</v>
       </c>
       <c r="M12" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="N12" s="52" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="45" t="s">
+        <v>343</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="C13" s="52" t="s">
         <v>369</v>
       </c>
-      <c r="N12" s="52" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
-        <v>344</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>370</v>
-      </c>
       <c r="D13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H13" s="50"/>
       <c r="K13" s="31"/>
     </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="45" t="s">
+        <v>371</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>353</v>
+      </c>
+      <c r="C15" s="31" t="s">
         <v>372</v>
       </c>
-      <c r="B15" s="37" t="s">
-        <v>354</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>373</v>
-      </c>
       <c r="D15" s="31" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16" s="49"/>
     </row>
-    <row r="22" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="14"/>
     </row>
-    <row r="23" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="54"/>
+    <row r="23" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C23" s="53"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
cuentas sit venta de equipos
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="398">
   <si>
     <t>Descripción</t>
   </si>
@@ -1031,9 +1031,6 @@
     <t>Cambio SimCard</t>
   </si>
   <si>
-    <t>59886002</t>
-  </si>
-  <si>
     <t>NARANJA</t>
   </si>
   <si>
@@ -1079,9 +1076,6 @@
     <t>Alta Linea Equip New AG</t>
   </si>
   <si>
-    <t>Homero Thompson</t>
-  </si>
-  <si>
     <t>Homero</t>
   </si>
   <si>
@@ -1097,9 +1091,6 @@
     <t>Habilitacion</t>
   </si>
   <si>
-    <t>26879334</t>
-  </si>
-  <si>
     <t>3413069797</t>
   </si>
   <si>
@@ -1151,9 +1142,6 @@
     <t>11120000000212</t>
   </si>
   <si>
-    <t>35653982</t>
-  </si>
-  <si>
     <t>18766558</t>
   </si>
   <si>
@@ -1167,13 +1155,79 @@
   </si>
   <si>
     <t>Femenino</t>
+  </si>
+  <si>
+    <t>cf@gmail.com</t>
+  </si>
+  <si>
+    <t>Centro de Servicio Santa Fe - Juan de Garay 444</t>
+  </si>
+  <si>
+    <t>Galaxy S8 - Negro</t>
+  </si>
+  <si>
+    <t>Bariloche</t>
+  </si>
+  <si>
+    <t>HSBC BANK ARGENTINA S.A.</t>
+  </si>
+  <si>
+    <t>Visa Crédito</t>
+  </si>
+  <si>
+    <t>5399099990081010</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>BBVA BANCO FRANCES SA</t>
+  </si>
+  <si>
+    <t>Visa Debito</t>
+  </si>
+  <si>
+    <t>4487790000000010</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Nombre Cuenta</t>
+  </si>
+  <si>
+    <t>Recargas TD</t>
+  </si>
+  <si>
+    <t>Río Negro</t>
+  </si>
+  <si>
+    <t>Alta Linea Existe OfCom Debito</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>4487790000000018</t>
+  </si>
+  <si>
+    <t>Neta Lyn Chang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1269,8 +1323,39 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
+      <color rgb="FF49739C"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF00396B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00396B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0070D2"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1405,7 +1490,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1476,14 +1561,22 @@
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -2103,10 +2196,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9:W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2119,11 +2212,14 @@
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
+    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="28.21875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2279,7 +2375,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D4">
         <v>52486595</v>
@@ -2345,13 +2441,13 @@
         <v>308</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C6" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D6" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="E6" t="s">
         <v>276</v>
@@ -2386,25 +2482,25 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B7">
-        <v>59886004</v>
+        <v>59886017</v>
       </c>
       <c r="C7" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D7" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="E7" t="s">
         <v>276</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="52">
         <v>32016</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="H7" t="s">
         <v>114</v>
@@ -2413,7 +2509,7 @@
         <v>280</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>324</v>
@@ -2425,28 +2521,28 @@
         <v>1524</v>
       </c>
       <c r="N7" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="O7" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="R7" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="O7" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="P7" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q7" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="R7" s="31" t="s">
+      <c r="S7" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="S7" s="31" t="s">
+      <c r="T7" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="T7" s="31" t="s">
+      <c r="U7" s="31" t="s">
         <v>340</v>
-      </c>
-      <c r="U7" s="31" t="s">
-        <v>341</v>
       </c>
       <c r="V7" s="31"/>
       <c r="W7" s="31"/>
@@ -2454,16 +2550,16 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="C8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D8" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E8" t="s">
         <v>276</v>
@@ -2472,7 +2568,7 @@
         <v>278</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H8" t="s">
         <v>114</v>
@@ -2495,97 +2591,97 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>349</v>
-      </c>
-      <c r="B9" s="32"/>
-      <c r="C9" t="s">
-        <v>366</v>
-      </c>
-      <c r="D9" t="s">
-        <v>367</v>
-      </c>
-      <c r="E9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>363</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>276</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="E9" s="31" t="s">
         <v>278</v>
       </c>
-      <c r="G9" s="33" t="s">
-        <v>353</v>
-      </c>
-      <c r="H9" t="s">
-        <v>114</v>
-      </c>
-      <c r="I9" t="s">
-        <v>322</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="K9" s="31" t="s">
+      <c r="F9" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>311</v>
+      </c>
+      <c r="I9" s="59" t="s">
+        <v>377</v>
+      </c>
+      <c r="J9" s="31" t="s">
+        <v>378</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>393</v>
+      </c>
+      <c r="L9" s="31" t="s">
+        <v>379</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="L9">
-        <v>1544</v>
-      </c>
-      <c r="M9">
-        <v>1524</v>
-      </c>
-      <c r="N9" s="41" t="s">
-        <v>337</v>
-      </c>
-      <c r="O9" s="31" t="s">
+      <c r="N9">
+        <v>666</v>
+      </c>
+      <c r="O9" s="59">
+        <v>666</v>
+      </c>
+      <c r="P9" s="59" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q9" s="59" t="s">
+        <v>381</v>
+      </c>
+      <c r="R9" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="P9" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="Q9" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="R9" s="31" t="s">
-        <v>338</v>
-      </c>
       <c r="S9" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="T9" s="31" t="s">
-        <v>340</v>
+        <v>341</v>
+      </c>
+      <c r="T9" s="60" t="s">
+        <v>382</v>
       </c>
       <c r="U9" s="31" t="s">
-        <v>341</v>
+        <v>383</v>
       </c>
       <c r="V9" s="31" t="s">
-        <v>302</v>
+        <v>384</v>
       </c>
       <c r="W9" s="31" t="s">
-        <v>334</v>
-      </c>
-      <c r="X9" s="46" t="s">
-        <v>350</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="X9" s="46"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="C10" s="51" t="s">
+        <v>373</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="E10" t="s">
+        <v>375</v>
+      </c>
+      <c r="F10" s="32" t="s">
+        <v>346</v>
+      </c>
+      <c r="G10" s="33" t="s">
         <v>345</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C10" s="52" t="s">
-        <v>377</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>378</v>
-      </c>
-      <c r="E10" t="s">
-        <v>379</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>347</v>
-      </c>
-      <c r="G10" s="33" t="s">
-        <v>346</v>
       </c>
       <c r="H10" t="s">
         <v>114</v>
@@ -2597,6 +2693,38 @@
         <v>323</v>
       </c>
       <c r="K10" s="49"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>395</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>396</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>2019</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>390</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2606,8 +2734,8 @@
     <hyperlink ref="G5" r:id="rId4"/>
     <hyperlink ref="G6" r:id="rId5"/>
     <hyperlink ref="G8" r:id="rId6"/>
-    <hyperlink ref="G9" r:id="rId7"/>
-    <hyperlink ref="G7" r:id="rId8"/>
+    <hyperlink ref="G7" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId9"/>
@@ -4453,8 +4581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4463,11 +4591,11 @@
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="5" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="11.5546875" customWidth="1"/>
+    <col min="9" max="13" width="11.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="16" max="26" width="9.109375" customWidth="1"/>
   </cols>
@@ -4565,34 +4693,34 @@
         <v>301</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>370</v>
+        <v>366</v>
+      </c>
+      <c r="C5" s="51" t="s">
+        <v>367</v>
       </c>
       <c r="D5" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>334</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="H5" s="31" t="s">
         <v>337</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="H5" s="31" t="s">
+      <c r="I5" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="J5" s="31" t="s">
         <v>339</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="K5" s="31" t="s">
         <v>340</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>341</v>
       </c>
       <c r="L5" s="31" t="s">
         <v>302</v>
@@ -4612,16 +4740,16 @@
         <v>315</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>370</v>
+        <v>366</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>367</v>
       </c>
       <c r="D6" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="E6" s="51" t="s">
-        <v>353</v>
+        <v>368</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4629,27 +4757,27 @@
         <v>316</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>370</v>
+        <v>366</v>
+      </c>
+      <c r="C7" s="51" t="s">
+        <v>367</v>
       </c>
       <c r="D7" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="E7" s="51" t="s">
-        <v>353</v>
+        <v>368</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="45" t="s">
         <v>317</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C8" s="52" t="s">
-        <v>370</v>
+      <c r="B8" s="62">
+        <v>19006577</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>397</v>
       </c>
       <c r="D8" s="47" t="s">
         <v>313</v>
@@ -4666,12 +4794,12 @@
         <v>319</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C9" s="42">
         <v>123</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="61">
         <v>1515151515</v>
       </c>
       <c r="E9" s="31"/>
@@ -4691,7 +4819,7 @@
         <v>320</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4699,7 +4827,7 @@
         <v>321</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4707,91 +4835,174 @@
         <v>333</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C12" s="52" t="s">
-        <v>370</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>337</v>
-      </c>
-      <c r="E12" s="31" t="s">
+        <v>366</v>
+      </c>
+      <c r="C12" s="51" t="s">
+        <v>367</v>
+      </c>
+      <c r="D12" s="59" t="s">
+        <v>380</v>
+      </c>
+      <c r="E12" s="59" t="s">
+        <v>381</v>
+      </c>
+      <c r="F12" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="F12" s="31" t="s">
-        <v>336</v>
-      </c>
       <c r="G12" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>338</v>
+        <v>341</v>
+      </c>
+      <c r="H12" s="60" t="s">
+        <v>382</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>339</v>
+        <v>383</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>340</v>
+        <v>384</v>
       </c>
       <c r="K12" s="31" t="s">
-        <v>341</v>
+        <v>385</v>
       </c>
       <c r="L12" s="31" t="s">
         <v>302</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="N12" s="52" t="s">
-        <v>377</v>
+        <v>366</v>
+      </c>
+      <c r="N12" s="51" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
-        <v>344</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>369</v>
-      </c>
-      <c r="C13" s="52" t="s">
-        <v>370</v>
-      </c>
-      <c r="D13" t="s">
         <v>343</v>
       </c>
-      <c r="H13" s="50"/>
-      <c r="K13" s="31"/>
+      <c r="B13" s="62">
+        <v>19006577</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="D13" s="59" t="s">
+        <v>380</v>
+      </c>
+      <c r="E13" s="59" t="s">
+        <v>381</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>341</v>
+      </c>
+      <c r="H13" s="60" t="s">
+        <v>382</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>383</v>
+      </c>
+      <c r="J13" s="31" t="s">
+        <v>384</v>
+      </c>
+      <c r="K13" s="31" t="s">
+        <v>385</v>
+      </c>
+      <c r="L13" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="M13" s="62">
+        <v>19006577</v>
+      </c>
+      <c r="N13" s="31" t="s">
+        <v>397</v>
+      </c>
+      <c r="O13" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
+        <v>369</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>352</v>
+      </c>
+      <c r="C15" s="31" t="s">
+        <v>370</v>
+      </c>
+      <c r="D15" s="31" t="s">
         <v>372</v>
       </c>
-      <c r="B15" s="37" t="s">
-        <v>354</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>373</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>376</v>
-      </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="49"/>
-    </row>
-    <row r="22" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>367</v>
+      </c>
+      <c r="D16" s="59" t="s">
+        <v>386</v>
+      </c>
+      <c r="E16" s="59" t="s">
+        <v>387</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="G16" s="60" t="s">
+        <v>388</v>
+      </c>
+      <c r="H16" s="31" t="s">
+        <v>389</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>384</v>
+      </c>
+      <c r="J16" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="K16" s="31" t="s">
+        <v>302</v>
+      </c>
+      <c r="L16" s="31">
+        <v>19784521</v>
+      </c>
+      <c r="M16" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="N16" s="31">
+        <v>3463406620</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="56"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="54"/>
+    </row>
+    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="58"/>
+      <c r="N20" s="63"/>
+    </row>
+    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="14"/>
-    </row>
-    <row r="23" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="54"/>
+      <c r="E22" s="49"/>
+    </row>
+    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="53"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Cuentas Sit y UAT 6  - 9
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15768" windowHeight="13152" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15768" windowHeight="13152" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Marketing" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="399">
   <si>
     <t>Descripción</t>
   </si>
@@ -866,9 +866,6 @@
     <t>08/08/1992</t>
   </si>
   <si>
-    <t>vicente lopez</t>
-  </si>
-  <si>
     <t>Buenos Aires</t>
   </si>
   <si>
@@ -941,9 +938,6 @@
     <t>Alta Linea Nuevo Agente Presencial</t>
   </si>
   <si>
-    <t>VICENTE LOPEZ</t>
-  </si>
-  <si>
     <t>Alta Linea Existente OfCom Presencial</t>
   </si>
   <si>
@@ -992,24 +986,12 @@
     <t>Suspension</t>
   </si>
   <si>
-    <t>Ajustes</t>
-  </si>
-  <si>
-    <t>Santa Fe</t>
-  </si>
-  <si>
-    <t>Rosario</t>
-  </si>
-  <si>
     <t>Falsa</t>
   </si>
   <si>
     <t>1524</t>
   </si>
   <si>
-    <t xml:space="preserve">Rosario </t>
-  </si>
-  <si>
     <t>aaaaaMalan</t>
   </si>
   <si>
@@ -1064,12 +1046,6 @@
     <t>Alta Linea Equipo Existe</t>
   </si>
   <si>
-    <t>llala</t>
-  </si>
-  <si>
-    <t>10/10/1992</t>
-  </si>
-  <si>
     <t>Alta Linea Equipo New OfCom</t>
   </si>
   <si>
@@ -1127,12 +1103,6 @@
     <t>Codi Aleatorio</t>
   </si>
   <si>
-    <t>15907314</t>
-  </si>
-  <si>
-    <t>Emma Valentina Miranda</t>
-  </si>
-  <si>
     <t>9900000766810001</t>
   </si>
   <si>
@@ -1142,19 +1112,82 @@
     <t>11120000000212</t>
   </si>
   <si>
-    <t>18766558</t>
+    <t>35653982</t>
   </si>
   <si>
     <t>0818</t>
   </si>
   <si>
-    <t>Emma Valentina</t>
-  </si>
-  <si>
-    <t>Miranda</t>
-  </si>
-  <si>
-    <t>Femenino</t>
+    <t>Río Negro</t>
+  </si>
+  <si>
+    <t>Bariloche</t>
+  </si>
+  <si>
+    <t>22222000</t>
+  </si>
+  <si>
+    <t>Cero Newton</t>
+  </si>
+  <si>
+    <t>2944675417</t>
+  </si>
+  <si>
+    <t>ceronewton@gmail.com</t>
+  </si>
+  <si>
+    <t>Newton</t>
+  </si>
+  <si>
+    <t>08/08/1993</t>
+  </si>
+  <si>
+    <t>22222001</t>
+  </si>
+  <si>
+    <t>22222002</t>
+  </si>
+  <si>
+    <t>22222003</t>
+  </si>
+  <si>
+    <t>22222004</t>
+  </si>
+  <si>
+    <t>22222005</t>
+  </si>
+  <si>
+    <t>22222006</t>
+  </si>
+  <si>
+    <t>22222008</t>
+  </si>
+  <si>
+    <t>5399099990081010</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>Alta Linea Existe OfCom Debito</t>
+  </si>
+  <si>
+    <t>BBVA BANCO FRANCES SA</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>4487790000000018</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>Alta Linea Equipo Existe OfCom Debito</t>
+  </si>
+  <si>
+    <t>Galaxy S8 - Negro</t>
   </si>
   <si>
     <t>cf@gmail.com</t>
@@ -1163,74 +1196,41 @@
     <t>Centro de Servicio Santa Fe - Juan de Garay 444</t>
   </si>
   <si>
-    <t>Galaxy S8 - Negro</t>
-  </si>
-  <si>
-    <t>Bariloche</t>
-  </si>
-  <si>
     <t>HSBC BANK ARGENTINA S.A.</t>
   </si>
   <si>
     <t>Visa Crédito</t>
   </si>
   <si>
-    <t>5399099990081010</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
     <t>2019</t>
   </si>
   <si>
-    <t>159</t>
-  </si>
-  <si>
-    <t>BBVA BANCO FRANCES SA</t>
-  </si>
-  <si>
-    <t>Visa Debito</t>
-  </si>
-  <si>
-    <t>4487790000000010</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>Nombre Cuenta</t>
-  </si>
-  <si>
-    <t>Recargas TD</t>
-  </si>
-  <si>
-    <t>Río Negro</t>
-  </si>
-  <si>
-    <t>Alta Linea Existe OfCom Debito</t>
-  </si>
-  <si>
-    <t>VISA</t>
-  </si>
-  <si>
-    <t>4487790000000018</t>
-  </si>
-  <si>
-    <t>Neta Lyn Chang</t>
-  </si>
-  <si>
-    <t>Alta Linea Equipo Existe OfCom Debito</t>
+    <t>Cuatro</t>
+  </si>
+  <si>
+    <t>Linea Equipo Existe SPU</t>
+  </si>
+  <si>
+    <t>Vicente Lopez</t>
+  </si>
+  <si>
+    <t>Ajustes REPRO</t>
+  </si>
+  <si>
+    <t>Ajustes PRE</t>
+  </si>
+  <si>
+    <t>Ocho Newton</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1261,14 +1261,17 @@
       <b/>
       <sz val="12"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1298,6 +1301,7 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1327,38 +1331,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF49739C"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF00396B"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00396B"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0070D2"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1493,7 +1466,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1554,9 +1527,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1565,21 +1536,22 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1919,7 +1891,7 @@
         <v>8</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -1967,7 +1939,7 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2068,7 @@
     </row>
     <row r="8" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B8" t="s">
         <v>274</v>
@@ -2114,72 +2086,72 @@
         <v>277</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
-        <v>280</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>304</v>
+        <v>363</v>
+      </c>
+      <c r="I8" t="s">
+        <v>364</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="31"/>
-      <c r="L8" s="43"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="31"/>
       <c r="N8" s="31"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>305</v>
-      </c>
-      <c r="B9" s="44">
-        <v>46534534</v>
+        <v>303</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>365</v>
       </c>
       <c r="C9" s="30" t="s">
-        <v>277</v>
+        <v>368</v>
       </c>
       <c r="D9" t="s">
-        <v>155</v>
+        <v>114</v>
       </c>
       <c r="E9" t="s">
-        <v>280</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>304</v>
+        <v>363</v>
+      </c>
+      <c r="F9" t="s">
+        <v>364</v>
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
       <c r="K9" s="31"/>
-      <c r="L9" s="43"/>
+      <c r="L9" s="42"/>
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="45" t="s">
-        <v>306</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>296</v>
-      </c>
-      <c r="C10" s="44">
-        <v>46534534</v>
-      </c>
-      <c r="D10" s="44">
-        <v>1158423198</v>
+      <c r="A10" s="43" t="s">
+        <v>304</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="D10" s="50" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="45" t="s">
-        <v>307</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>300</v>
-      </c>
-      <c r="C11" s="44">
-        <v>23444455</v>
-      </c>
-      <c r="D11" s="44">
-        <v>1158423198</v>
+      <c r="A11" s="43" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>365</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -2187,9 +2159,10 @@
     <hyperlink ref="G8" r:id="rId1" display="malannominacion@gmail.com"/>
     <hyperlink ref="F8" r:id="rId2"/>
     <hyperlink ref="D9" r:id="rId3" display="malannominacion@gmail.com"/>
+    <hyperlink ref="C9" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPágina &amp;P</oddFooter>
@@ -2199,15 +2172,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.109375" customWidth="1"/>
     <col min="4" max="5" width="19.44140625" customWidth="1"/>
@@ -2215,14 +2188,11 @@
     <col min="7" max="7" width="26" customWidth="1"/>
     <col min="8" max="8" width="22.33203125" customWidth="1"/>
     <col min="9" max="9" width="26" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" customWidth="1"/>
-    <col min="20" max="20" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2251,13 +2221,13 @@
         <v>48</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>282</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>283</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>49</v>
@@ -2283,13 +2253,13 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C2" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D2" t="s">
         <v>275</v>
@@ -2307,31 +2277,31 @@
         <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>322</v>
+        <v>363</v>
       </c>
       <c r="J2" t="s">
-        <v>323</v>
+        <v>364</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="N2" s="31" t="s">
+        <v>307</v>
+      </c>
+      <c r="O2" s="42" t="s">
+        <v>308</v>
+      </c>
+      <c r="P2" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="O2" s="43" t="s">
+      <c r="Q2" s="31" t="s">
         <v>310</v>
-      </c>
-      <c r="P2" s="31" t="s">
-        <v>311</v>
-      </c>
-      <c r="Q2" s="31" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -2339,13 +2309,13 @@
         <v>76</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" t="s">
         <v>284</v>
-      </c>
-      <c r="D3" t="s">
-        <v>285</v>
       </c>
       <c r="E3" t="s">
         <v>276</v>
@@ -2360,10 +2330,10 @@
         <v>114</v>
       </c>
       <c r="I3" t="s">
-        <v>280</v>
+        <v>363</v>
       </c>
       <c r="J3" t="s">
-        <v>279</v>
+        <v>364</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="32"/>
@@ -2378,7 +2348,7 @@
         <v>29</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D4">
         <v>52486595</v>
@@ -2401,56 +2371,56 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>285</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" t="s">
         <v>286</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>292</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>287</v>
-      </c>
-      <c r="D5" t="s">
-        <v>288</v>
       </c>
       <c r="E5" t="s">
         <v>276</v>
       </c>
       <c r="F5" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="G5" s="30" t="s">
         <v>289</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>290</v>
       </c>
       <c r="H5" t="s">
         <v>114</v>
       </c>
       <c r="I5" t="s">
-        <v>280</v>
+        <v>363</v>
       </c>
       <c r="J5" t="s">
-        <v>279</v>
+        <v>364</v>
       </c>
       <c r="K5" s="32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M5" s="32"/>
       <c r="N5" s="32"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="C6" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="D6" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E6" t="s">
         <v>276</v>
@@ -2465,104 +2435,104 @@
         <v>114</v>
       </c>
       <c r="I6" t="s">
-        <v>322</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>326</v>
+        <v>363</v>
+      </c>
+      <c r="J6" t="s">
+        <v>364</v>
       </c>
       <c r="K6" s="31" t="s">
+        <v>307</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>308</v>
+      </c>
+      <c r="M6" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="L6" s="43" t="s">
+      <c r="N6" s="31" t="s">
         <v>310</v>
-      </c>
-      <c r="M6" s="31" t="s">
-        <v>311</v>
-      </c>
-      <c r="N6" s="31" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B7">
-        <v>59886017</v>
+        <v>59886004</v>
       </c>
       <c r="C7" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="D7" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="E7" t="s">
         <v>276</v>
       </c>
-      <c r="F7" s="52">
-        <v>32016</v>
+      <c r="F7" s="31" t="s">
+        <v>288</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="H7" t="s">
         <v>114</v>
       </c>
       <c r="I7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="L7">
-        <v>1524</v>
-      </c>
-      <c r="M7">
-        <v>1524</v>
+        <v>319</v>
+      </c>
+      <c r="L7" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>320</v>
       </c>
       <c r="N7" s="41" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="O7" s="31" t="s">
+        <v>328</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="R7" s="31" t="s">
+        <v>331</v>
+      </c>
+      <c r="S7" s="31" t="s">
+        <v>332</v>
+      </c>
+      <c r="T7" s="31" t="s">
+        <v>333</v>
+      </c>
+      <c r="U7" s="31" t="s">
         <v>334</v>
-      </c>
-      <c r="P7" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q7" s="31" t="s">
-        <v>341</v>
-      </c>
-      <c r="R7" s="31" t="s">
-        <v>337</v>
-      </c>
-      <c r="S7" s="31" t="s">
-        <v>338</v>
-      </c>
-      <c r="T7" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="U7" s="31" t="s">
-        <v>340</v>
       </c>
       <c r="V7" s="31"/>
       <c r="W7" s="31"/>
-      <c r="X7" s="46"/>
+      <c r="X7" s="44"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="C8" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="D8" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="E8" t="s">
         <v>276</v>
@@ -2571,19 +2541,19 @@
         <v>278</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="H8" t="s">
         <v>114</v>
       </c>
       <c r="I8" t="s">
-        <v>322</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>323</v>
+        <v>363</v>
+      </c>
+      <c r="J8" t="s">
+        <v>364</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="L8">
         <v>1524</v>
@@ -2594,13 +2564,13 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>276</v>
@@ -2608,116 +2578,116 @@
       <c r="E9" s="31" t="s">
         <v>278</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>376</v>
+      <c r="F9" s="48" t="s">
+        <v>387</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>310</v>
-      </c>
-      <c r="H9" s="59" t="s">
-        <v>311</v>
-      </c>
-      <c r="I9" s="59" t="s">
-        <v>377</v>
+        <v>308</v>
+      </c>
+      <c r="H9" s="56" t="s">
+        <v>309</v>
+      </c>
+      <c r="I9" s="56" t="s">
+        <v>388</v>
       </c>
       <c r="J9" s="31" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>393</v>
+        <v>363</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>379</v>
+        <v>364</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="N9">
         <v>666</v>
       </c>
-      <c r="O9" s="59">
+      <c r="O9" s="56">
         <v>666</v>
       </c>
-      <c r="P9" s="59" t="s">
-        <v>380</v>
-      </c>
-      <c r="Q9" s="59" t="s">
-        <v>381</v>
+      <c r="P9" s="56" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q9" s="56" t="s">
+        <v>390</v>
       </c>
       <c r="R9" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="S9" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="S9" s="31" t="s">
-        <v>341</v>
-      </c>
-      <c r="T9" s="60" t="s">
-        <v>382</v>
+      <c r="T9" s="57" t="s">
+        <v>378</v>
       </c>
       <c r="U9" s="31" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="V9" s="31" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="W9" s="31" t="s">
-        <v>385</v>
-      </c>
-      <c r="X9" s="46"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+        <v>379</v>
+      </c>
+      <c r="X9" s="58"/>
+    </row>
+    <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>366</v>
-      </c>
-      <c r="C10" s="51" t="s">
-        <v>373</v>
+        <v>338</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>374</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>393</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="E10" t="s">
-        <v>375</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>346</v>
+        <v>369</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>370</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>345</v>
+        <v>368</v>
       </c>
       <c r="H10" t="s">
         <v>114</v>
       </c>
       <c r="I10" t="s">
-        <v>322</v>
+        <v>363</v>
       </c>
       <c r="J10" t="s">
-        <v>323</v>
-      </c>
-      <c r="K10" s="49"/>
+        <v>364</v>
+      </c>
+      <c r="K10" s="47"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>394</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>366</v>
+        <v>380</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>374</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>114</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2726,30 +2696,30 @@
         <v>2019</v>
       </c>
       <c r="J11" s="31" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>366</v>
+        <v>385</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>374</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>378</v>
+        <v>386</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2758,7 +2728,27 @@
         <v>2019</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>390</v>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>394</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>374</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>386</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -2770,10 +2760,11 @@
     <hyperlink ref="G6" r:id="rId5"/>
     <hyperlink ref="G8" r:id="rId6"/>
     <hyperlink ref="G7" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="G10" r:id="rId8"/>
+    <hyperlink ref="F9" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -2958,7 +2949,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3032,13 +3023,13 @@
         <v>19</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -4614,10 +4605,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:Z26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4626,11 +4617,11 @@
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="13" width="11.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="11.5546875" customWidth="1"/>
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
     <col min="16" max="26" width="9.109375" customWidth="1"/>
   </cols>
@@ -4643,13 +4634,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -4675,16 +4666,16 @@
     </row>
     <row r="2" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B2" s="38">
         <v>46534534</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E2" s="39">
         <v>1158423198</v>
@@ -4695,7 +4686,7 @@
     </row>
     <row r="3" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B3" s="36">
         <v>23444455</v>
@@ -4706,136 +4697,136 @@
         <v>1161138552</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="B4" s="38">
-        <v>46534534</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>365</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>366</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>298</v>
-      </c>
-      <c r="E4" s="39">
-        <v>1158423198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>371</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>389</v>
+      </c>
+      <c r="E5" s="56" t="s">
+        <v>390</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>335</v>
+      </c>
+      <c r="H5" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="I5" s="31" t="s">
+        <v>391</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>379</v>
+      </c>
+      <c r="L5" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>366</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>367</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>336</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>334</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>341</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>337</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>338</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>339</v>
-      </c>
-      <c r="K5" s="31" t="s">
-        <v>340</v>
-      </c>
-      <c r="L5" s="31" t="s">
-        <v>302</v>
-      </c>
-      <c r="M5" s="31">
-        <v>19784521</v>
+      <c r="M5" s="54" t="s">
+        <v>365</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="O5" s="31">
         <v>3463406620</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>313</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>372</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>358</v>
+      </c>
+      <c r="E6" s="48" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="43" t="s">
+        <v>314</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>358</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="43" t="s">
         <v>315</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B8" s="51" t="s">
+        <v>374</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>366</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="D8" s="45" t="s">
+        <v>311</v>
+      </c>
+      <c r="E8" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="F8" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>375</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D9" s="50" t="s">
         <v>367</v>
-      </c>
-      <c r="D6" s="47" t="s">
-        <v>368</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="45" t="s">
-        <v>316</v>
-      </c>
-      <c r="B7" s="37" t="s">
-        <v>366</v>
-      </c>
-      <c r="C7" s="51" t="s">
-        <v>367</v>
-      </c>
-      <c r="D7" s="47" t="s">
-        <v>368</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
-        <v>317</v>
-      </c>
-      <c r="B8" s="62">
-        <v>19006577</v>
-      </c>
-      <c r="C8" s="31" t="s">
-        <v>397</v>
-      </c>
-      <c r="D8" s="47" t="s">
-        <v>313</v>
-      </c>
-      <c r="E8" s="48" t="s">
-        <v>314</v>
-      </c>
-      <c r="F8" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>319</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>366</v>
-      </c>
-      <c r="C9" s="42">
-        <v>123</v>
-      </c>
-      <c r="D9" s="61">
-        <v>1515151515</v>
       </c>
       <c r="E9" s="31"/>
       <c r="F9" s="31"/>
@@ -4849,195 +4840,158 @@
       <c r="N9" s="31"/>
       <c r="O9" s="14"/>
     </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
-        <v>320</v>
-      </c>
-      <c r="B10" s="37" t="s">
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="43" t="s">
+        <v>318</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>376</v>
+      </c>
+      <c r="C10" s="50" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
-        <v>321</v>
-      </c>
-      <c r="B11" s="37" t="s">
+    <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="43" t="s">
+        <v>397</v>
+      </c>
+      <c r="B11" s="54" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="45" t="s">
-        <v>333</v>
-      </c>
-      <c r="B12" s="37" t="s">
+      <c r="C11" s="50" t="s">
         <v>366</v>
       </c>
-      <c r="C12" s="51" t="s">
-        <v>367</v>
-      </c>
-      <c r="D12" s="59" t="s">
-        <v>380</v>
-      </c>
-      <c r="E12" s="59" t="s">
-        <v>381</v>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="43" t="s">
+        <v>327</v>
+      </c>
+      <c r="B12" s="54" t="s">
+        <v>377</v>
+      </c>
+      <c r="C12" s="50" t="s">
+        <v>366</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>389</v>
+      </c>
+      <c r="E12" s="56" t="s">
+        <v>390</v>
       </c>
       <c r="F12" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="G12" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="G12" s="31" t="s">
-        <v>341</v>
-      </c>
-      <c r="H12" s="60" t="s">
-        <v>382</v>
+      <c r="H12" s="57" t="s">
+        <v>378</v>
       </c>
       <c r="I12" s="31" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="J12" s="31" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="K12" s="31" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="L12" s="31" t="s">
-        <v>302</v>
-      </c>
-      <c r="M12" s="37" t="s">
+        <v>301</v>
+      </c>
+      <c r="M12" s="54" t="s">
+        <v>377</v>
+      </c>
+      <c r="N12" s="50" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="43" t="s">
+        <v>337</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>377</v>
+      </c>
+      <c r="C13" s="53" t="s">
         <v>366</v>
       </c>
-      <c r="N12" s="51" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="45" t="s">
-        <v>343</v>
-      </c>
-      <c r="B13" s="62">
-        <v>19006577</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>397</v>
-      </c>
-      <c r="D13" s="59" t="s">
-        <v>380</v>
-      </c>
-      <c r="E13" s="59" t="s">
-        <v>381</v>
+      <c r="D13" s="56" t="s">
+        <v>389</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>390</v>
       </c>
       <c r="F13" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="G13" s="31" t="s">
         <v>335</v>
       </c>
-      <c r="G13" s="31" t="s">
-        <v>341</v>
-      </c>
-      <c r="H13" s="60" t="s">
-        <v>382</v>
+      <c r="H13" s="57" t="s">
+        <v>378</v>
       </c>
       <c r="I13" s="31" t="s">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>384</v>
+        <v>392</v>
       </c>
       <c r="K13" s="31" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>302</v>
-      </c>
-      <c r="M13" s="62">
-        <v>19006577</v>
-      </c>
-      <c r="N13" s="31" t="s">
-        <v>397</v>
+        <v>301</v>
+      </c>
+      <c r="M13" s="52" t="s">
+        <v>377</v>
+      </c>
+      <c r="N13" s="50" t="s">
+        <v>398</v>
       </c>
       <c r="O13" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
-        <v>353</v>
+      <c r="A14" s="43" t="s">
+        <v>345</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="45" t="s">
-        <v>369</v>
+      <c r="A15" s="43" t="s">
+        <v>359</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>392</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>366</v>
-      </c>
-      <c r="C16" s="51" t="s">
-        <v>367</v>
-      </c>
-      <c r="D16" s="59" t="s">
-        <v>386</v>
-      </c>
-      <c r="E16" s="59" t="s">
-        <v>387</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="G16" s="60" t="s">
-        <v>388</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>389</v>
-      </c>
-      <c r="I16" s="31" t="s">
-        <v>384</v>
-      </c>
-      <c r="J16" s="31" t="s">
-        <v>390</v>
-      </c>
-      <c r="K16" s="31" t="s">
-        <v>302</v>
-      </c>
-      <c r="L16" s="31">
-        <v>19784521</v>
-      </c>
-      <c r="M16" s="31" t="s">
-        <v>391</v>
-      </c>
-      <c r="N16" s="31">
-        <v>3463406620</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="54"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="58"/>
-      <c r="N20" s="63"/>
-    </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="43" t="s">
+        <v>396</v>
+      </c>
+      <c r="B16">
+        <v>22222000</v>
+      </c>
+      <c r="E16" s="47"/>
+    </row>
+    <row r="22" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="14"/>
-      <c r="E22" s="49"/>
-    </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="53"/>
+    </row>
+    <row r="23" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="49"/>
+    </row>
+    <row r="26" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="47"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Las cuentas en amarillo
</commit_message>
<xml_diff>
--- a/Cuentas.xlsx
+++ b/Cuentas.xlsx
@@ -1275,13 +1275,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1361,6 +1354,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF49739C"/>
       <name val="Arial"/>
@@ -1398,7 +1398,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1421,6 +1421,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1513,36 +1519,180 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1550,79 +1700,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1630,90 +1712,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1722,7 +1720,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1730,8 +1728,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1758,8 +1768,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="21" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1842,9 +1852,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1948,9 +1958,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2021,10 +2031,10 @@
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="7"/>
@@ -2033,7 +2043,7 @@
       <c r="A5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="11" t="s">
         <v>21</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -2044,7 +2054,7 @@
       <c r="A6" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="0" t="n">
@@ -2058,7 +2068,7 @@
       <c r="A7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="0" t="n">
@@ -2081,10 +2091,10 @@
       <c r="D8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>31</v>
       </c>
       <c r="G8" s="0" t="s">
@@ -2093,23 +2103,23 @@
       <c r="H8" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="15"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="17" t="n">
+      <c r="B9" s="16" t="n">
         <v>46534534</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>31</v>
       </c>
       <c r="D9" s="0" t="s">
@@ -2118,41 +2128,41 @@
       <c r="E9" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="17" t="n">
+      <c r="C10" s="16" t="n">
         <v>46534534</v>
       </c>
-      <c r="D10" s="17" t="n">
+      <c r="D10" s="16" t="n">
         <v>1158423198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="17" t="n">
+      <c r="C11" s="16" t="n">
         <v>23444455</v>
       </c>
-      <c r="D11" s="17" t="n">
+      <c r="D11" s="16" t="n">
         <v>1158423198</v>
       </c>
     </row>
@@ -2186,7 +2196,7 @@
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="19.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.33"/>
@@ -2195,15 +2205,15 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="28.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="17.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2266,7 +2276,7 @@
       <c r="A2" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -2278,10 +2288,10 @@
       <c r="E2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="13" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="0" t="s">
@@ -2293,25 +2303,25 @@
       <c r="J2" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="13" t="s">
+      <c r="N2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="12" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2319,7 +2329,7 @@
       <c r="A3" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -2331,10 +2341,10 @@
       <c r="E3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="0" t="s">
@@ -2346,10 +2356,10 @@
       <c r="J3" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -2358,7 +2368,7 @@
       <c r="B4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>70</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -2373,10 +2383,10 @@
       <c r="G4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2384,7 +2394,7 @@
       <c r="A5" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C5" s="0" t="s">
@@ -2396,10 +2406,10 @@
       <c r="E5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>76</v>
       </c>
       <c r="H5" s="0" t="s">
@@ -2411,20 +2421,20 @@
       <c r="J5" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>79</v>
       </c>
       <c r="C6" s="0" t="s">
@@ -2436,10 +2446,10 @@
       <c r="E6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>31</v>
       </c>
       <c r="H6" s="0" t="s">
@@ -2448,24 +2458,24 @@
       <c r="I6" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="K6" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="L6" s="16" t="s">
+      <c r="L6" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="M6" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="N6" s="12" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>83</v>
       </c>
       <c r="B7" s="0" t="n">
@@ -2480,10 +2490,10 @@
       <c r="E7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="20" t="n">
+      <c r="F7" s="19" t="n">
         <v>32016</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>86</v>
       </c>
       <c r="H7" s="0" t="s">
@@ -2492,10 +2502,10 @@
       <c r="I7" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="14" t="s">
         <v>58</v>
       </c>
       <c r="L7" s="0" t="n">
@@ -2504,39 +2514,39 @@
       <c r="M7" s="0" t="n">
         <v>1524</v>
       </c>
-      <c r="N7" s="21" t="s">
+      <c r="N7" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="O7" s="13" t="s">
+      <c r="O7" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="P7" s="13" t="s">
+      <c r="P7" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="Q7" s="13" t="s">
+      <c r="Q7" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="R7" s="13" t="s">
+      <c r="R7" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="S7" s="13" t="s">
+      <c r="S7" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="T7" s="13" t="s">
+      <c r="T7" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="22"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>97</v>
       </c>
       <c r="C8" s="0" t="s">
@@ -2548,10 +2558,10 @@
       <c r="E8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>100</v>
       </c>
       <c r="H8" s="0" t="s">
@@ -2560,10 +2570,10 @@
       <c r="I8" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J8" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="14" t="s">
         <v>58</v>
       </c>
       <c r="L8" s="0" t="n">
@@ -2574,97 +2584,97 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="M9" s="15" t="s">
+      <c r="M9" s="14" t="s">
         <v>58</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>666</v>
       </c>
-      <c r="O9" s="24" t="n">
+      <c r="O9" s="23" t="n">
         <v>666</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="P9" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="Q9" s="24" t="s">
+      <c r="Q9" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="R9" s="13" t="s">
+      <c r="R9" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="S9" s="13" t="s">
+      <c r="S9" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="T9" s="25" t="s">
+      <c r="T9" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="U9" s="13" t="s">
+      <c r="U9" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="V9" s="13" t="s">
+      <c r="V9" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="W9" s="13" t="s">
+      <c r="W9" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="X9" s="22"/>
+      <c r="X9" s="21"/>
     </row>
     <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>118</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>121</v>
       </c>
       <c r="H10" s="0" t="s">
@@ -2676,28 +2686,28 @@
       <c r="J10" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="K10" s="28"/>
+      <c r="K10" s="27"/>
     </row>
     <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G11" s="12" t="s">
         <v>126</v>
       </c>
       <c r="H11" s="0" t="n">
@@ -2706,30 +2716,30 @@
       <c r="I11" s="0" t="n">
         <v>2019</v>
       </c>
-      <c r="J11" s="13" t="s">
+      <c r="J11" s="12" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>126</v>
       </c>
       <c r="H12" s="0" t="n">
@@ -2738,7 +2748,7 @@
       <c r="I12" s="0" t="n">
         <v>2019</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2777,31 +2787,31 @@
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>134</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -2813,12 +2823,12 @@
       <c r="D2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="29" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B3" s="0" t="s">
@@ -2827,15 +2837,15 @@
       <c r="C3" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="15" t="n">
+      <c r="D3" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="29" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="0" t="s">
@@ -2844,44 +2854,44 @@
       <c r="C4" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="15" t="n">
+      <c r="D4" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="29" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>140</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="15" t="n">
+      <c r="D5" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="29" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>140</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="D6" s="15" t="n">
+      <c r="D6" s="14" t="n">
         <v>10</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="29" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2912,9 +2922,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2991,9 +3001,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="5" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="14" min="5" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="15" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3073,9 +3083,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.89"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="11.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="14" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="4" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="14" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3155,9 +3165,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="38.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="40.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="10.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="40.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3173,22 +3183,22 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="30" t="s">
         <v>156</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>157</v>
       </c>
       <c r="K1" s="5"/>
@@ -3209,572 +3219,572 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D2" s="32" t="n">
+      <c r="D2" s="31" t="n">
         <v>3413104291</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="F2" s="34" t="n">
+      <c r="F2" s="33" t="n">
         <v>722341170199331</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="31" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="32" t="n">
+      <c r="D3" s="31" t="n">
         <v>3413104292</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="F3" s="34" t="n">
+      <c r="F3" s="33" t="n">
         <v>722341170199332</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="31" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D4" s="32" t="n">
+      <c r="D4" s="31" t="n">
         <v>3413104293</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="F4" s="34" t="n">
+      <c r="F4" s="33" t="n">
         <v>722341170199333</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="31" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D5" s="32" t="n">
+      <c r="D5" s="31" t="n">
         <v>3413104294</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="F5" s="34" t="n">
+      <c r="F5" s="33" t="n">
         <v>722341170199334</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="31" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D6" s="32" t="n">
+      <c r="D6" s="31" t="n">
         <v>3413104295</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="F6" s="34" t="n">
+      <c r="F6" s="33" t="n">
         <v>722341170199335</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="31" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D7" s="32" t="n">
+      <c r="D7" s="31" t="n">
         <v>3413104296</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="F7" s="34" t="n">
+      <c r="F7" s="33" t="n">
         <v>722341170199336</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="31" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D8" s="32" t="n">
+      <c r="D8" s="31" t="n">
         <v>3413104297</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="F8" s="34" t="n">
+      <c r="F8" s="33" t="n">
         <v>722341170199337</v>
       </c>
-      <c r="G8" s="32" t="s">
+      <c r="G8" s="31" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D9" s="32" t="n">
+      <c r="D9" s="31" t="n">
         <v>3413104298</v>
       </c>
-      <c r="E9" s="33" t="s">
+      <c r="E9" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="F9" s="34" t="n">
+      <c r="F9" s="33" t="n">
         <v>722341170199338</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="31" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="32" t="n">
+      <c r="D10" s="31" t="n">
         <v>3413104299</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="F10" s="34" t="n">
+      <c r="F10" s="33" t="n">
         <v>722341170199339</v>
       </c>
-      <c r="G10" s="32" t="s">
+      <c r="G10" s="31" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D11" s="32" t="n">
+      <c r="D11" s="31" t="n">
         <v>3413104300</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="32" t="s">
         <v>178</v>
       </c>
-      <c r="F11" s="34" t="n">
+      <c r="F11" s="33" t="n">
         <v>722341170199340</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="31" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D12" s="32" t="n">
+      <c r="D12" s="31" t="n">
         <v>3413104301</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="32" t="s">
         <v>181</v>
       </c>
-      <c r="F12" s="34" t="n">
+      <c r="F12" s="33" t="n">
         <v>722341170199341</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="31" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D13" s="32" t="n">
+      <c r="D13" s="31" t="n">
         <v>3413104302</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="F13" s="34" t="n">
+      <c r="F13" s="33" t="n">
         <v>722341170199342</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="31" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D14" s="32" t="n">
+      <c r="D14" s="31" t="n">
         <v>3413104303</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="F14" s="34" t="n">
+      <c r="F14" s="33" t="n">
         <v>722341170199343</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="31" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D15" s="32" t="n">
+      <c r="D15" s="31" t="n">
         <v>3413104304</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="F15" s="34" t="n">
+      <c r="F15" s="33" t="n">
         <v>722341170199344</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="31" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="32" t="n">
+      <c r="D16" s="31" t="n">
         <v>3413104305</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="F16" s="34" t="n">
+      <c r="F16" s="33" t="n">
         <v>722341170199345</v>
       </c>
-      <c r="G16" s="32" t="s">
+      <c r="G16" s="31" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D17" s="32" t="n">
+      <c r="D17" s="31" t="n">
         <v>3413104306</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="F17" s="34" t="n">
+      <c r="F17" s="33" t="n">
         <v>722341170199346</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="31" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D18" s="32" t="n">
+      <c r="D18" s="31" t="n">
         <v>3413104307</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="F18" s="34" t="n">
+      <c r="F18" s="33" t="n">
         <v>722341170199347</v>
       </c>
-      <c r="G18" s="32" t="s">
+      <c r="G18" s="31" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D19" s="32" t="n">
+      <c r="D19" s="31" t="n">
         <v>3413104308</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="F19" s="34" t="n">
+      <c r="F19" s="33" t="n">
         <v>722341170199348</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="31" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D20" s="32" t="n">
+      <c r="D20" s="31" t="n">
         <v>3413104309</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="F20" s="34" t="n">
+      <c r="F20" s="33" t="n">
         <v>722341170199349</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="G20" s="31" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D21" s="32" t="n">
+      <c r="D21" s="31" t="n">
         <v>3413104310</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="F21" s="34" t="n">
+      <c r="F21" s="33" t="n">
         <v>722341170199350</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="31" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D22" s="15" t="n">
+      <c r="D22" s="14" t="n">
         <v>3413104311</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="F22" s="34" t="n">
+      <c r="F22" s="33" t="n">
         <v>722341170199351</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="G22" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="I22" s="34" t="n">
+      <c r="I22" s="33" t="n">
         <v>722341170199353</v>
       </c>
-      <c r="J22" s="15" t="s">
+      <c r="J22" s="14" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="D23" s="15" t="n">
+      <c r="D23" s="14" t="n">
         <v>3413104312</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="32" t="s">
         <v>206</v>
       </c>
-      <c r="F23" s="34" t="n">
+      <c r="F23" s="33" t="n">
         <v>722341170199352</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="I23" s="34" t="n">
+      <c r="I23" s="33" t="n">
         <v>722341170199354</v>
       </c>
-      <c r="J23" s="15" t="s">
+      <c r="J23" s="14" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D24" s="15" t="n">
+      <c r="D24" s="14" t="n">
         <v>3413104313</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="F24" s="34" t="n">
+      <c r="F24" s="33" t="n">
         <v>722341170199355</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="14" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>180</v>
       </c>
-      <c r="D25" s="15" t="n">
+      <c r="D25" s="14" t="n">
         <v>3413104314</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="F25" s="34" t="n">
+      <c r="F25" s="33" t="n">
         <v>722341170199356</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="14" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3782,7 +3792,7 @@
       <c r="A26" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="0" t="n">
@@ -3793,741 +3803,741 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="E27" s="35" t="s">
+      <c r="E27" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="F27" s="35" t="s">
+      <c r="F27" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="G27" s="35" t="s">
+      <c r="G27" s="34" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="34" t="s">
         <v>220</v>
       </c>
-      <c r="F28" s="35" t="s">
+      <c r="F28" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="G28" s="35" t="s">
+      <c r="G28" s="34" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="34" t="s">
         <v>223</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="34" t="s">
         <v>224</v>
       </c>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="34" t="s">
         <v>225</v>
       </c>
-      <c r="G29" s="35" t="s">
+      <c r="G29" s="34" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="34" t="s">
         <v>228</v>
       </c>
-      <c r="F30" s="35" t="s">
+      <c r="F30" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="G30" s="35" t="s">
+      <c r="G30" s="34" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="34" t="s">
         <v>232</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="G31" s="35" t="s">
+      <c r="G31" s="34" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E32" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="F32" s="35" t="s">
+      <c r="F32" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="G32" s="35" t="s">
+      <c r="G32" s="34" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C33" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="F33" s="35" t="s">
+      <c r="F33" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="G33" s="34" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C34" s="35" t="s">
+      <c r="C34" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="F34" s="35" t="s">
+      <c r="F34" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="G34" s="35" t="s">
+      <c r="G34" s="34" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="15" t="s">
+      <c r="A35" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="34" t="s">
         <v>247</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E35" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="F35" s="35" t="s">
+      <c r="F35" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="G35" s="35" t="s">
+      <c r="G35" s="34" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E36" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="F36" s="35" t="s">
+      <c r="F36" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="G36" s="35" t="s">
+      <c r="G36" s="34" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D37" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="F37" s="35" t="s">
+      <c r="F37" s="34" t="s">
         <v>257</v>
       </c>
-      <c r="G37" s="35" t="s">
+      <c r="G37" s="34" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C38" s="35" t="s">
+      <c r="C38" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="34" t="s">
         <v>259</v>
       </c>
-      <c r="E38" s="35" t="s">
+      <c r="E38" s="34" t="s">
         <v>260</v>
       </c>
-      <c r="F38" s="35" t="s">
+      <c r="F38" s="34" t="s">
         <v>261</v>
       </c>
-      <c r="G38" s="35" t="s">
+      <c r="G38" s="34" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C39" s="35" t="s">
+      <c r="C39" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="34" t="s">
         <v>263</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="34" t="s">
         <v>264</v>
       </c>
-      <c r="F39" s="35" t="s">
+      <c r="F39" s="34" t="s">
         <v>265</v>
       </c>
-      <c r="G39" s="35" t="s">
+      <c r="G39" s="34" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C40" s="35" t="s">
+      <c r="C40" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="34" t="s">
         <v>267</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="34" t="s">
         <v>268</v>
       </c>
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="34" t="s">
         <v>269</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="G40" s="34" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C41" s="35" t="s">
+      <c r="C41" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="34" t="s">
         <v>272</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="34" t="s">
         <v>273</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="G41" s="34" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C42" s="35" t="s">
+      <c r="C42" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D42" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="E42" s="35" t="s">
+      <c r="E42" s="34" t="s">
         <v>276</v>
       </c>
-      <c r="F42" s="35" t="s">
+      <c r="F42" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="G42" s="35" t="s">
+      <c r="G42" s="34" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C43" s="35" t="s">
+      <c r="C43" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="34" t="s">
         <v>279</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="34" t="s">
         <v>280</v>
       </c>
-      <c r="F43" s="35" t="s">
+      <c r="F43" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="G43" s="35" t="s">
+      <c r="G43" s="34" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="34" t="s">
         <v>283</v>
       </c>
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="34" t="s">
         <v>284</v>
       </c>
-      <c r="F44" s="35" t="s">
+      <c r="F44" s="34" t="s">
         <v>285</v>
       </c>
-      <c r="G44" s="35" t="s">
+      <c r="G44" s="34" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C45" s="35" t="s">
+      <c r="C45" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="35" t="s">
+      <c r="D45" s="34" t="s">
         <v>287</v>
       </c>
-      <c r="E45" s="35" t="s">
+      <c r="E45" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="F45" s="35" t="s">
+      <c r="F45" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="G45" s="35" t="s">
+      <c r="G45" s="34" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C46" s="35" t="s">
+      <c r="C46" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="35" t="s">
+      <c r="D46" s="34" t="s">
         <v>291</v>
       </c>
-      <c r="E46" s="35" t="s">
+      <c r="E46" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="F46" s="35" t="s">
+      <c r="F46" s="34" t="s">
         <v>293</v>
       </c>
-      <c r="G46" s="35" t="s">
+      <c r="G46" s="34" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C47" s="35" t="s">
+      <c r="C47" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D47" s="35" t="s">
+      <c r="D47" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="E47" s="35" t="s">
+      <c r="E47" s="34" t="s">
         <v>296</v>
       </c>
-      <c r="F47" s="35" t="s">
+      <c r="F47" s="34" t="s">
         <v>297</v>
       </c>
-      <c r="G47" s="35" t="s">
+      <c r="G47" s="34" t="s">
         <v>298</v>
       </c>
-      <c r="H47" s="35" t="s">
+      <c r="H47" s="34" t="s">
         <v>299</v>
       </c>
-      <c r="I47" s="35" t="s">
+      <c r="I47" s="34" t="s">
         <v>300</v>
       </c>
-      <c r="J47" s="35" t="s">
+      <c r="J47" s="34" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C48" s="35" t="s">
+      <c r="C48" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="35" t="s">
+      <c r="D48" s="34" t="s">
         <v>302</v>
       </c>
-      <c r="E48" s="35" t="s">
+      <c r="E48" s="34" t="s">
         <v>303</v>
       </c>
-      <c r="F48" s="35" t="s">
+      <c r="F48" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="G48" s="35" t="s">
+      <c r="G48" s="34" t="s">
         <v>305</v>
       </c>
-      <c r="H48" s="35" t="s">
+      <c r="H48" s="34" t="s">
         <v>306</v>
       </c>
-      <c r="I48" s="35" t="s">
+      <c r="I48" s="34" t="s">
         <v>307</v>
       </c>
-      <c r="J48" s="35" t="s">
+      <c r="J48" s="34" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C49" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D49" s="34" t="s">
         <v>310</v>
       </c>
-      <c r="E49" s="35" t="s">
+      <c r="E49" s="34" t="s">
         <v>311</v>
       </c>
-      <c r="F49" s="35" t="s">
+      <c r="F49" s="34" t="s">
         <v>312</v>
       </c>
-      <c r="G49" s="35" t="s">
+      <c r="G49" s="34" t="s">
         <v>313</v>
       </c>
-      <c r="H49" s="35" t="s">
+      <c r="H49" s="34" t="s">
         <v>314</v>
       </c>
-      <c r="I49" s="35" t="s">
+      <c r="I49" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="J49" s="35" t="s">
+      <c r="J49" s="34" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C50" s="35" t="s">
+      <c r="C50" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="E50" s="35" t="s">
+      <c r="E50" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="F50" s="35" t="s">
+      <c r="F50" s="34" t="s">
         <v>319</v>
       </c>
-      <c r="G50" s="35" t="s">
+      <c r="G50" s="34" t="s">
         <v>320</v>
       </c>
-      <c r="H50" s="35" t="s">
+      <c r="H50" s="34" t="s">
         <v>321</v>
       </c>
-      <c r="I50" s="35" t="s">
+      <c r="I50" s="34" t="s">
         <v>322</v>
       </c>
-      <c r="J50" s="35" t="s">
+      <c r="J50" s="34" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C51" s="35" t="s">
+      <c r="C51" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="34" t="s">
         <v>324</v>
       </c>
-      <c r="E51" s="35" t="s">
+      <c r="E51" s="34" t="s">
         <v>325</v>
       </c>
-      <c r="F51" s="35" t="s">
+      <c r="F51" s="34" t="s">
         <v>326</v>
       </c>
-      <c r="G51" s="35" t="s">
+      <c r="G51" s="34" t="s">
         <v>327</v>
       </c>
-      <c r="H51" s="35" t="s">
+      <c r="H51" s="34" t="s">
         <v>328</v>
       </c>
-      <c r="I51" s="35" t="s">
+      <c r="I51" s="34" t="s">
         <v>329</v>
       </c>
-      <c r="J51" s="35" t="s">
+      <c r="J51" s="34" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="35" t="s">
+      <c r="D52" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="E52" s="35" t="s">
+      <c r="E52" s="34" t="s">
         <v>332</v>
       </c>
-      <c r="F52" s="35" t="s">
+      <c r="F52" s="34" t="s">
         <v>333</v>
       </c>
-      <c r="G52" s="35" t="s">
+      <c r="G52" s="34" t="s">
         <v>334</v>
       </c>
-      <c r="H52" s="35" t="s">
+      <c r="H52" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="I52" s="35" t="s">
+      <c r="I52" s="34" t="s">
         <v>336</v>
       </c>
-      <c r="J52" s="35" t="s">
+      <c r="J52" s="34" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="35" t="s">
+      <c r="D53" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="E53" s="35" t="s">
+      <c r="E53" s="34" t="s">
         <v>339</v>
       </c>
-      <c r="F53" s="35" t="s">
+      <c r="F53" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="G53" s="35" t="s">
+      <c r="G53" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="H53" s="35" t="s">
+      <c r="H53" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="I53" s="35" t="s">
+      <c r="I53" s="34" t="s">
         <v>343</v>
       </c>
-      <c r="J53" s="35" t="s">
+      <c r="J53" s="34" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="35" t="s">
+      <c r="D54" s="34" t="s">
         <v>345</v>
       </c>
-      <c r="E54" s="35" t="s">
+      <c r="E54" s="34" t="s">
         <v>346</v>
       </c>
-      <c r="F54" s="35" t="s">
+      <c r="F54" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="G54" s="35" t="s">
+      <c r="G54" s="34" t="s">
         <v>348</v>
       </c>
-      <c r="H54" s="35" t="s">
+      <c r="H54" s="34" t="s">
         <v>349</v>
       </c>
-      <c r="I54" s="35" t="s">
+      <c r="I54" s="34" t="s">
         <v>350</v>
       </c>
-      <c r="J54" s="35" t="s">
+      <c r="J54" s="34" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="14" t="s">
         <v>352</v>
       </c>
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C55" s="35" t="s">
+      <c r="C55" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D55" s="35" t="s">
+      <c r="D55" s="34" t="s">
         <v>353</v>
       </c>
-      <c r="E55" s="35" t="s">
+      <c r="E55" s="34" t="s">
         <v>354</v>
       </c>
-      <c r="F55" s="35" t="s">
+      <c r="F55" s="34" t="s">
         <v>355</v>
       </c>
-      <c r="G55" s="35" t="s">
+      <c r="G55" s="34" t="s">
         <v>356</v>
       </c>
       <c r="H55" s="0" t="n">
@@ -4535,25 +4545,25 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="14" t="s">
         <v>352</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="34" t="s">
         <v>214</v>
       </c>
-      <c r="C56" s="35" t="s">
+      <c r="C56" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="35" t="s">
+      <c r="D56" s="34" t="s">
         <v>357</v>
       </c>
-      <c r="E56" s="35" t="s">
+      <c r="E56" s="34" t="s">
         <v>358</v>
       </c>
-      <c r="F56" s="35" t="s">
+      <c r="F56" s="34" t="s">
         <v>359</v>
       </c>
-      <c r="G56" s="35" t="s">
+      <c r="G56" s="34" t="s">
         <v>360</v>
       </c>
       <c r="H56" s="0" t="n">
@@ -4561,63 +4571,63 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="14" t="s">
         <v>361</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="34" t="s">
         <v>362</v>
       </c>
-      <c r="C57" s="35" t="s">
+      <c r="C57" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="35" t="n">
+      <c r="D57" s="34" t="n">
         <v>2213104354</v>
       </c>
-      <c r="E57" s="35" t="n">
+      <c r="E57" s="34" t="n">
         <v>895434</v>
       </c>
-      <c r="F57" s="35" t="n">
+      <c r="F57" s="34" t="n">
         <v>72234</v>
       </c>
-      <c r="G57" s="35" t="s">
+      <c r="G57" s="34" t="s">
         <v>363</v>
       </c>
-      <c r="H57" s="36" t="s">
+      <c r="H57" s="35" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="34" t="s">
         <v>362</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C58" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D58" s="35" t="n">
+      <c r="D58" s="34" t="n">
         <v>2213104355</v>
       </c>
-      <c r="E58" s="35" t="n">
+      <c r="E58" s="34" t="n">
         <v>895435</v>
       </c>
-      <c r="F58" s="35" t="n">
+      <c r="F58" s="34" t="n">
         <v>72235</v>
       </c>
-      <c r="G58" s="37" t="s">
+      <c r="G58" s="36" t="s">
         <v>366</v>
       </c>
-      <c r="H58" s="38" t="s">
+      <c r="H58" s="37" t="s">
         <v>364</v>
       </c>
-      <c r="I58" s="39" t="n">
+      <c r="I58" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="J58" s="38" t="s">
+      <c r="J58" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="K58" s="40" t="n">
+      <c r="K58" s="39" t="n">
         <v>523654</v>
       </c>
     </row>
@@ -4640,7 +4650,7 @@
   <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4649,14 +4659,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="19.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.11"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="9" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="9" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="16" style="0" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="16" style="0" width="9.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4669,10 +4679,10 @@
       <c r="C1" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>369</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="41" t="s">
         <v>370</v>
       </c>
       <c r="F1" s="4"/>
@@ -4698,19 +4708,19 @@
       <c r="Z1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="43" t="n">
+      <c r="B2" s="42" t="n">
         <v>46534534</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>371</v>
       </c>
-      <c r="E2" s="44" t="n">
+      <c r="E2" s="42" t="n">
         <v>1158423198</v>
       </c>
       <c r="F2" s="0" t="n">
@@ -4718,130 +4728,130 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="45" t="n">
+      <c r="B3" s="43" t="n">
         <v>23444455</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="21"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="20"/>
       <c r="G3" s="0" t="n">
         <v>1161138552</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="43" t="n">
+      <c r="B4" s="42" t="n">
         <v>46534534</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>371</v>
       </c>
-      <c r="E4" s="44" t="n">
+      <c r="E4" s="42" t="n">
         <v>1158423198</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="M5" s="13" t="n">
+      <c r="M5" s="12" t="n">
         <v>19784521</v>
       </c>
-      <c r="N5" s="13" t="s">
+      <c r="N5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="O5" s="13" t="n">
+      <c r="O5" s="12" t="n">
         <v>3463406620</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="45" t="s">
         <v>376</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>377</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="45" t="s">
         <v>376</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="B8" s="48" t="n">
+      <c r="B8" s="46" t="n">
         <v>19006577</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="D8" s="47" t="s">
+      <c r="D8" s="45" t="s">
         <v>380</v>
       </c>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="47" t="s">
         <v>381</v>
       </c>
       <c r="F8" s="0" t="s">
@@ -4849,131 +4859,131 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="50" t="n">
+      <c r="C9" s="48" t="n">
         <v>123</v>
       </c>
-      <c r="D9" s="51" t="n">
+      <c r="D9" s="49" t="n">
         <v>1515151515</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="15"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="50" t="s">
         <v>385</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>386</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="M12" s="26" t="s">
+      <c r="M12" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="N12" s="27" t="s">
+      <c r="N12" s="26" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="17" t="s">
         <v>387</v>
       </c>
-      <c r="B13" s="48" t="n">
+      <c r="B13" s="46" t="n">
         <v>19006577</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="M13" s="48" t="n">
+      <c r="M13" s="46" t="n">
         <v>19006577</v>
       </c>
-      <c r="N13" s="13" t="s">
+      <c r="N13" s="12" t="s">
         <v>379</v>
       </c>
       <c r="O13" s="0" t="s">
@@ -4981,73 +4991,73 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>389</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>392</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>394</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="23" t="s">
         <v>124</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="23" t="s">
         <v>396</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="I16" s="13" t="s">
+      <c r="I16" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="J16" s="13" t="s">
+      <c r="J16" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="L16" s="13" t="n">
+      <c r="L16" s="12" t="n">
         <v>19784521</v>
       </c>
-      <c r="M16" s="13" t="s">
+      <c r="M16" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="N16" s="13" t="n">
+      <c r="N16" s="12" t="n">
         <v>3463406620</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="50" t="s">
         <v>400</v>
       </c>
       <c r="B17" s="0" t="n">
@@ -5055,7 +5065,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="51" t="s">
         <v>401</v>
       </c>
       <c r="B18" s="52" t="n">
@@ -5063,24 +5073,24 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="53" t="s">
         <v>402</v>
       </c>
       <c r="B19" s="52" t="n">
         <v>19006577</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="51" t="s">
         <v>403</v>
       </c>
       <c r="B20" s="52" t="n">
         <v>10777540</v>
       </c>
-      <c r="D20" s="55"/>
-      <c r="N20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="N20" s="57"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>